<commit_message>
->update download template daily log day and night
</commit_message>
<xml_diff>
--- a/StarEnergi/App_Data/daily_log/DailyLogDay_BaseTemplate.xlsx
+++ b/StarEnergi/App_Data/daily_log/DailyLogDay_BaseTemplate.xlsx
@@ -427,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="89">
+  <borders count="94">
     <border>
       <left/>
       <right/>
@@ -1466,24 +1466,97 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
       <top style="hair">
         <color indexed="64"/>
       </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="double">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -1504,7 +1577,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="227">
+  <cellXfs count="220">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1584,9 +1657,6 @@
     <xf numFmtId="2" fontId="8" fillId="5" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="4" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="8" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1594,9 +1664,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="19" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1604,9 +1671,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="16" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="19" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1737,28 +1801,6 @@
     <xf numFmtId="2" fontId="8" fillId="6" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="25" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="11" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="54" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="12" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1783,213 +1825,12 @@
     <xf numFmtId="2" fontId="8" fillId="6" borderId="22" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="27" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="2" borderId="69" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="2" borderId="14" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="2" borderId="88" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="69" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="70" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="71" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="72" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="73" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="74" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="75" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="76" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="67" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="68" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="77" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="78" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="79" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="80" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="81" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="82" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="39" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="83" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="10" fillId="0" borderId="84" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="86" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="67" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="56" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="62" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="8" fillId="5" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="8" fillId="5" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="61" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="4" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -2031,6 +1872,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2071,12 +1915,224 @@
     <xf numFmtId="4" fontId="8" fillId="5" borderId="61" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="46" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="83" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="3" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="3" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="3" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="77" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="78" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="79" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="80" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="81" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="82" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="39" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="83" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="84" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="86" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="67" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="2" borderId="69" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="2" borderId="14" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="2" borderId="87" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="69" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="70" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="71" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="72" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="73" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="74" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="75" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="76" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="67" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="68" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="56" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="62" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="61" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="59" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="89" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="91" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="92" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="92" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2481,15 +2537,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A4" zoomScale="93" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:C9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="93" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="100"/>
+    <col min="1" max="1" width="9.140625" style="97"/>
     <col min="2" max="2" width="9.140625" style="6"/>
-    <col min="3" max="3" width="9.140625" style="101"/>
+    <col min="3" max="3" width="9.140625" style="98"/>
     <col min="4" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -2512,36 +2568,36 @@
     <row r="2" spans="1:14">
       <c r="A2" s="7"/>
       <c r="B2" s="8"/>
-      <c r="C2" s="140" t="s">
+      <c r="C2" s="157" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="140"/>
-      <c r="E2" s="140"/>
-      <c r="F2" s="140"/>
-      <c r="G2" s="140"/>
-      <c r="H2" s="140"/>
-      <c r="I2" s="140"/>
-      <c r="J2" s="140"/>
-      <c r="K2" s="140"/>
-      <c r="L2" s="140"/>
-      <c r="M2" s="140"/>
-      <c r="N2" s="141"/>
+      <c r="D2" s="157"/>
+      <c r="E2" s="157"/>
+      <c r="F2" s="157"/>
+      <c r="G2" s="157"/>
+      <c r="H2" s="157"/>
+      <c r="I2" s="157"/>
+      <c r="J2" s="157"/>
+      <c r="K2" s="157"/>
+      <c r="L2" s="157"/>
+      <c r="M2" s="157"/>
+      <c r="N2" s="158"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="9"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="140"/>
-      <c r="H3" s="140"/>
-      <c r="I3" s="140"/>
-      <c r="J3" s="140"/>
-      <c r="K3" s="140"/>
-      <c r="L3" s="140"/>
-      <c r="M3" s="140"/>
-      <c r="N3" s="141"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="157"/>
+      <c r="I3" s="157"/>
+      <c r="J3" s="157"/>
+      <c r="K3" s="157"/>
+      <c r="L3" s="157"/>
+      <c r="M3" s="157"/>
+      <c r="N3" s="158"/>
     </row>
     <row r="4" spans="1:14" ht="19.5">
       <c r="A4" s="9"/>
@@ -2598,108 +2654,108 @@
       <c r="N6" s="16"/>
     </row>
     <row r="7" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A7" s="142" t="s">
+      <c r="A7" s="159" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="143"/>
-      <c r="C7" s="144"/>
+      <c r="B7" s="160"/>
+      <c r="C7" s="161"/>
       <c r="D7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="145" t="s">
+      <c r="E7" s="162" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="144"/>
-      <c r="G7" s="145" t="s">
+      <c r="F7" s="161"/>
+      <c r="G7" s="162" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="143"/>
-      <c r="I7" s="143"/>
-      <c r="J7" s="143"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="143"/>
-      <c r="M7" s="143"/>
-      <c r="N7" s="146"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="160"/>
+      <c r="K7" s="160"/>
+      <c r="L7" s="160"/>
+      <c r="M7" s="160"/>
+      <c r="N7" s="163"/>
     </row>
     <row r="8" spans="1:14" ht="13.5" customHeight="1" thickTop="1">
-      <c r="A8" s="147">
+      <c r="A8" s="164">
         <v>41459</v>
       </c>
-      <c r="B8" s="148"/>
-      <c r="C8" s="149"/>
-      <c r="D8" s="153"/>
-      <c r="E8" s="155"/>
-      <c r="F8" s="156"/>
-      <c r="G8" s="159"/>
-      <c r="H8" s="160"/>
-      <c r="I8" s="159"/>
-      <c r="J8" s="160"/>
-      <c r="K8" s="159"/>
-      <c r="L8" s="160"/>
-      <c r="M8" s="164"/>
-      <c r="N8" s="165"/>
+      <c r="B8" s="165"/>
+      <c r="C8" s="166"/>
+      <c r="D8" s="170"/>
+      <c r="E8" s="172"/>
+      <c r="F8" s="173"/>
+      <c r="G8" s="176"/>
+      <c r="H8" s="177"/>
+      <c r="I8" s="176"/>
+      <c r="J8" s="177"/>
+      <c r="K8" s="176"/>
+      <c r="L8" s="177"/>
+      <c r="M8" s="178"/>
+      <c r="N8" s="179"/>
     </row>
     <row r="9" spans="1:14" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A9" s="150"/>
-      <c r="B9" s="151"/>
-      <c r="C9" s="152"/>
-      <c r="D9" s="154"/>
-      <c r="E9" s="157"/>
-      <c r="F9" s="158"/>
-      <c r="G9" s="166"/>
-      <c r="H9" s="167"/>
-      <c r="I9" s="166"/>
-      <c r="J9" s="167"/>
-      <c r="K9" s="166"/>
-      <c r="L9" s="167"/>
-      <c r="M9" s="168"/>
-      <c r="N9" s="169"/>
+      <c r="A9" s="167"/>
+      <c r="B9" s="168"/>
+      <c r="C9" s="169"/>
+      <c r="D9" s="171"/>
+      <c r="E9" s="174"/>
+      <c r="F9" s="175"/>
+      <c r="G9" s="180"/>
+      <c r="H9" s="181"/>
+      <c r="I9" s="180"/>
+      <c r="J9" s="181"/>
+      <c r="K9" s="180"/>
+      <c r="L9" s="181"/>
+      <c r="M9" s="182"/>
+      <c r="N9" s="183"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="130" t="s">
+      <c r="A10" s="187" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="189" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="133"/>
-      <c r="D10" s="133"/>
-      <c r="E10" s="133"/>
-      <c r="F10" s="133"/>
-      <c r="G10" s="133"/>
-      <c r="H10" s="133"/>
-      <c r="I10" s="133"/>
-      <c r="J10" s="133"/>
-      <c r="K10" s="133"/>
-      <c r="L10" s="133"/>
-      <c r="M10" s="133"/>
-      <c r="N10" s="134"/>
+      <c r="C10" s="190"/>
+      <c r="D10" s="190"/>
+      <c r="E10" s="190"/>
+      <c r="F10" s="190"/>
+      <c r="G10" s="190"/>
+      <c r="H10" s="190"/>
+      <c r="I10" s="190"/>
+      <c r="J10" s="190"/>
+      <c r="K10" s="190"/>
+      <c r="L10" s="190"/>
+      <c r="M10" s="190"/>
+      <c r="N10" s="191"/>
     </row>
     <row r="11" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A11" s="131"/>
-      <c r="B11" s="135" t="s">
+      <c r="A11" s="188"/>
+      <c r="B11" s="192" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="136"/>
-      <c r="D11" s="136"/>
-      <c r="E11" s="136"/>
-      <c r="F11" s="136"/>
-      <c r="G11" s="136"/>
-      <c r="H11" s="136"/>
-      <c r="I11" s="136"/>
-      <c r="J11" s="137" t="s">
+      <c r="C11" s="193"/>
+      <c r="D11" s="193"/>
+      <c r="E11" s="193"/>
+      <c r="F11" s="193"/>
+      <c r="G11" s="193"/>
+      <c r="H11" s="193"/>
+      <c r="I11" s="193"/>
+      <c r="J11" s="194" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="138"/>
-      <c r="L11" s="138"/>
-      <c r="M11" s="138"/>
-      <c r="N11" s="139"/>
+      <c r="K11" s="195"/>
+      <c r="L11" s="195"/>
+      <c r="M11" s="195"/>
+      <c r="N11" s="196"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="127">
+      <c r="A12" s="184">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B12" s="161" t="s">
+      <c r="B12" s="197" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="19" t="s">
@@ -2711,7 +2767,7 @@
       <c r="E12" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="161" t="s">
+      <c r="F12" s="197" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="20" t="s">
@@ -2734,8 +2790,8 @@
       <c r="N12" s="24"/>
     </row>
     <row r="13" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A13" s="128"/>
-      <c r="B13" s="162"/>
+      <c r="A13" s="185"/>
+      <c r="B13" s="198"/>
       <c r="C13" s="25" t="s">
         <v>17</v>
       </c>
@@ -2745,7 +2801,7 @@
       <c r="E13" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="163"/>
+      <c r="F13" s="199"/>
       <c r="G13" s="26" t="s">
         <v>17</v>
       </c>
@@ -2766,7 +2822,7 @@
       <c r="N13" s="29"/>
     </row>
     <row r="14" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A14" s="128"/>
+      <c r="A14" s="185"/>
       <c r="B14" s="30"/>
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
@@ -2774,15 +2830,15 @@
       <c r="F14" s="30"/>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="221"/>
-      <c r="K14" s="222"/>
-      <c r="L14" s="118"/>
+      <c r="I14" s="212"/>
+      <c r="J14" s="213"/>
+      <c r="K14" s="214"/>
+      <c r="L14" s="107"/>
       <c r="M14" s="32"/>
       <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
-      <c r="A15" s="128"/>
+      <c r="A15" s="185"/>
       <c r="B15" s="35"/>
       <c r="C15" s="31"/>
       <c r="D15" s="31"/>
@@ -2790,31 +2846,31 @@
       <c r="F15" s="35"/>
       <c r="G15" s="36"/>
       <c r="H15" s="31"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="223"/>
-      <c r="K15" s="224"/>
-      <c r="L15" s="119"/>
+      <c r="I15" s="215"/>
+      <c r="J15" s="211"/>
+      <c r="K15" s="210"/>
+      <c r="L15" s="108"/>
       <c r="M15" s="31"/>
-      <c r="N15" s="38"/>
+      <c r="N15" s="37"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1">
-      <c r="A16" s="128"/>
+      <c r="A16" s="185"/>
       <c r="B16" s="35"/>
-      <c r="C16" s="105"/>
-      <c r="D16" s="105"/>
-      <c r="E16" s="104"/>
+      <c r="C16" s="102"/>
+      <c r="D16" s="102"/>
+      <c r="E16" s="101"/>
       <c r="F16" s="35"/>
       <c r="G16" s="31"/>
       <c r="H16" s="31"/>
-      <c r="I16" s="37"/>
-      <c r="J16" s="223"/>
-      <c r="K16" s="224"/>
-      <c r="L16" s="120"/>
+      <c r="I16" s="215"/>
+      <c r="J16" s="209"/>
+      <c r="K16" s="210"/>
+      <c r="L16" s="109"/>
       <c r="M16" s="31"/>
-      <c r="N16" s="38"/>
+      <c r="N16" s="37"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="128"/>
+      <c r="A17" s="185"/>
       <c r="B17" s="35"/>
       <c r="C17" s="31"/>
       <c r="D17" s="31"/>
@@ -2822,15 +2878,15 @@
       <c r="F17" s="35"/>
       <c r="G17" s="31"/>
       <c r="H17" s="31"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="223"/>
-      <c r="K17" s="224"/>
-      <c r="L17" s="120"/>
+      <c r="I17" s="215"/>
+      <c r="J17" s="209"/>
+      <c r="K17" s="210"/>
+      <c r="L17" s="109"/>
       <c r="M17" s="31"/>
-      <c r="N17" s="38"/>
+      <c r="N17" s="37"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="128"/>
+      <c r="A18" s="185"/>
       <c r="B18" s="35"/>
       <c r="C18" s="31"/>
       <c r="D18" s="31"/>
@@ -2838,15 +2894,15 @@
       <c r="F18" s="35"/>
       <c r="G18" s="31"/>
       <c r="H18" s="31"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="223"/>
-      <c r="K18" s="224"/>
-      <c r="L18" s="121"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="38"/>
+      <c r="I18" s="215"/>
+      <c r="J18" s="209"/>
+      <c r="K18" s="210"/>
+      <c r="L18" s="110"/>
+      <c r="M18" s="38"/>
+      <c r="N18" s="37"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="128"/>
+      <c r="A19" s="185"/>
       <c r="B19" s="35"/>
       <c r="C19" s="31"/>
       <c r="D19" s="31"/>
@@ -2854,712 +2910,657 @@
       <c r="F19" s="35"/>
       <c r="G19" s="31"/>
       <c r="H19" s="31"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="223"/>
-      <c r="K19" s="224"/>
-      <c r="L19" s="120"/>
+      <c r="I19" s="215"/>
+      <c r="J19" s="209"/>
+      <c r="K19" s="210"/>
+      <c r="L19" s="109"/>
       <c r="M19" s="31"/>
-      <c r="N19" s="38"/>
+      <c r="N19" s="37"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="128"/>
+      <c r="A20" s="185"/>
       <c r="B20" s="35"/>
       <c r="C20" s="31"/>
       <c r="D20" s="31"/>
       <c r="E20" s="31"/>
-      <c r="F20" s="40"/>
+      <c r="F20" s="39"/>
       <c r="G20" s="31"/>
       <c r="H20" s="31"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="223"/>
-      <c r="K20" s="224"/>
-      <c r="L20" s="120"/>
+      <c r="I20" s="215"/>
+      <c r="J20" s="209"/>
+      <c r="K20" s="210"/>
+      <c r="L20" s="109"/>
       <c r="M20" s="31"/>
-      <c r="N20" s="38"/>
+      <c r="N20" s="37"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="128"/>
+      <c r="A21" s="185"/>
       <c r="B21" s="35"/>
       <c r="C21" s="31"/>
       <c r="D21" s="31"/>
       <c r="E21" s="31"/>
-      <c r="F21" s="40"/>
+      <c r="F21" s="39"/>
       <c r="G21" s="36"/>
       <c r="H21" s="36"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="223"/>
-      <c r="K21" s="224"/>
-      <c r="L21" s="120"/>
+      <c r="I21" s="215"/>
+      <c r="J21" s="209"/>
+      <c r="K21" s="210"/>
+      <c r="L21" s="109"/>
       <c r="M21" s="31"/>
-      <c r="N21" s="38"/>
+      <c r="N21" s="37"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="128"/>
+      <c r="A22" s="185"/>
       <c r="B22" s="35"/>
-      <c r="C22" s="106"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="42"/>
+      <c r="C22" s="103"/>
+      <c r="D22" s="103"/>
+      <c r="E22" s="103"/>
+      <c r="F22" s="40"/>
       <c r="G22" s="36"/>
       <c r="H22" s="36"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="223"/>
-      <c r="K22" s="224"/>
-      <c r="L22" s="120"/>
+      <c r="I22" s="215"/>
+      <c r="J22" s="209"/>
+      <c r="K22" s="210"/>
+      <c r="L22" s="109"/>
       <c r="M22" s="31"/>
-      <c r="N22" s="38"/>
+      <c r="N22" s="37"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="128"/>
+      <c r="A23" s="185"/>
       <c r="B23" s="35"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
       <c r="E23" s="31"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="223"/>
-      <c r="K23" s="224"/>
-      <c r="L23" s="120"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="215"/>
+      <c r="J23" s="209"/>
+      <c r="K23" s="210"/>
+      <c r="L23" s="109"/>
       <c r="M23" s="31"/>
-      <c r="N23" s="38"/>
+      <c r="N23" s="37"/>
     </row>
     <row r="24" spans="1:14" ht="15">
-      <c r="A24" s="128"/>
+      <c r="A24" s="185"/>
       <c r="B24" s="35"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
       <c r="E24" s="31"/>
-      <c r="F24" s="40"/>
-      <c r="G24" s="107"/>
-      <c r="H24" s="108"/>
-      <c r="I24" s="110"/>
-      <c r="J24" s="223"/>
-      <c r="K24" s="224"/>
-      <c r="L24" s="120"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="104"/>
+      <c r="H24" s="105"/>
+      <c r="I24" s="215"/>
+      <c r="J24" s="209"/>
+      <c r="K24" s="210"/>
+      <c r="L24" s="109"/>
       <c r="M24" s="31"/>
-      <c r="N24" s="38"/>
+      <c r="N24" s="37"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="128"/>
+      <c r="A25" s="185"/>
       <c r="B25" s="35"/>
-      <c r="C25" s="46"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="31"/>
-      <c r="E25" s="46"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="35"/>
-      <c r="G25" s="109"/>
-      <c r="H25" s="109"/>
-      <c r="I25" s="111"/>
-      <c r="J25" s="223"/>
-      <c r="K25" s="224"/>
-      <c r="L25" s="120"/>
+      <c r="G25" s="106"/>
+      <c r="H25" s="106"/>
+      <c r="I25" s="215"/>
+      <c r="J25" s="209"/>
+      <c r="K25" s="210"/>
+      <c r="L25" s="109"/>
       <c r="M25" s="31"/>
-      <c r="N25" s="38"/>
+      <c r="N25" s="37"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="128"/>
+      <c r="A26" s="185"/>
       <c r="B26" s="35"/>
-      <c r="C26" s="46"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="31"/>
-      <c r="E26" s="46"/>
+      <c r="E26" s="43"/>
       <c r="F26" s="35"/>
-      <c r="G26" s="102"/>
-      <c r="H26" s="103"/>
-      <c r="I26" s="112"/>
-      <c r="J26" s="223"/>
-      <c r="K26" s="224"/>
-      <c r="L26" s="120"/>
+      <c r="G26" s="99"/>
+      <c r="H26" s="100"/>
+      <c r="I26" s="215"/>
+      <c r="J26" s="209"/>
+      <c r="K26" s="210"/>
+      <c r="L26" s="109"/>
       <c r="M26" s="31"/>
-      <c r="N26" s="38"/>
+      <c r="N26" s="37"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="128"/>
-      <c r="B27" s="47"/>
-      <c r="C27" s="46"/>
+      <c r="A27" s="185"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="43"/>
       <c r="D27" s="31"/>
       <c r="E27" s="31"/>
       <c r="F27" s="35"/>
-      <c r="G27" s="102"/>
-      <c r="H27" s="103"/>
-      <c r="I27" s="112"/>
-      <c r="J27" s="223"/>
-      <c r="K27" s="224"/>
-      <c r="L27" s="120"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="100"/>
+      <c r="I27" s="215"/>
+      <c r="J27" s="209"/>
+      <c r="K27" s="210"/>
+      <c r="L27" s="109"/>
       <c r="M27" s="31"/>
-      <c r="N27" s="38"/>
+      <c r="N27" s="37"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="128"/>
+      <c r="A28" s="185"/>
       <c r="B28" s="35"/>
       <c r="C28" s="36"/>
       <c r="D28" s="32"/>
       <c r="E28" s="33"/>
-      <c r="F28" s="124"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="125"/>
-      <c r="I28" s="126"/>
-      <c r="J28" s="223"/>
-      <c r="K28" s="224"/>
-      <c r="L28" s="120"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="114"/>
+      <c r="H28" s="114"/>
+      <c r="I28" s="215"/>
+      <c r="J28" s="209"/>
+      <c r="K28" s="210"/>
+      <c r="L28" s="109"/>
       <c r="M28" s="31"/>
-      <c r="N28" s="38"/>
+      <c r="N28" s="37"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="128"/>
-      <c r="B29" s="48" t="s">
+      <c r="A29" s="185"/>
+      <c r="B29" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="48" t="s">
+      <c r="D29" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="48" t="s">
+      <c r="F29" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="48" t="s">
+      <c r="G29" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="48" t="s">
+      <c r="H29" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="48" t="s">
+      <c r="I29" s="216" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="223"/>
-      <c r="K29" s="224"/>
-      <c r="L29" s="120"/>
+      <c r="J29" s="211"/>
+      <c r="K29" s="210"/>
+      <c r="L29" s="109"/>
       <c r="M29" s="31"/>
-      <c r="N29" s="38"/>
+      <c r="N29" s="37"/>
     </row>
     <row r="30" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A30" s="128"/>
-      <c r="B30" s="49" t="s">
+      <c r="A30" s="185"/>
+      <c r="B30" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="49" t="s">
+      <c r="C30" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="49" t="s">
+      <c r="E30" s="46" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="49" t="s">
+      <c r="F30" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="49" t="s">
+      <c r="G30" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="49" t="s">
+      <c r="H30" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="113" t="s">
+      <c r="I30" s="217" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="223"/>
-      <c r="K30" s="224"/>
-      <c r="L30" s="120"/>
+      <c r="J30" s="211"/>
+      <c r="K30" s="210"/>
+      <c r="L30" s="109"/>
       <c r="M30" s="31"/>
-      <c r="N30" s="38"/>
+      <c r="N30" s="37"/>
     </row>
     <row r="31" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A31" s="128"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="114"/>
-      <c r="J31" s="223"/>
-      <c r="K31" s="224"/>
-      <c r="L31" s="122"/>
-      <c r="M31" s="46"/>
-      <c r="N31" s="38"/>
+      <c r="A31" s="185"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="47"/>
+      <c r="G31" s="47"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="218"/>
+      <c r="J31" s="211"/>
+      <c r="K31" s="210"/>
+      <c r="L31" s="111"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="37"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="128"/>
-      <c r="B32" s="51" t="s">
+      <c r="A32" s="185"/>
+      <c r="B32" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="52" t="s">
+      <c r="C32" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="48" t="s">
+      <c r="D32" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="48" t="s">
+      <c r="E32" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="48" t="s">
+      <c r="F32" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="48" t="s">
+      <c r="G32" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="H32" s="48" t="s">
+      <c r="H32" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="I32" s="115" t="s">
+      <c r="I32" s="216" t="s">
         <v>41</v>
       </c>
-      <c r="J32" s="223"/>
-      <c r="K32" s="224"/>
-      <c r="L32" s="120"/>
+      <c r="J32" s="211"/>
+      <c r="K32" s="210"/>
+      <c r="L32" s="109"/>
       <c r="M32" s="31"/>
-      <c r="N32" s="38"/>
+      <c r="N32" s="37"/>
     </row>
     <row r="33" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A33" s="128"/>
-      <c r="B33" s="49" t="s">
+      <c r="A33" s="185"/>
+      <c r="B33" s="46" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="49" t="s">
+      <c r="C33" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="49" t="s">
+      <c r="D33" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="49" t="s">
+      <c r="E33" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="49" t="s">
+      <c r="F33" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="49" t="s">
+      <c r="G33" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="H33" s="53" t="s">
+      <c r="H33" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="I33" s="116" t="s">
+      <c r="I33" s="219" t="s">
         <v>42</v>
       </c>
-      <c r="J33" s="223"/>
-      <c r="K33" s="224"/>
-      <c r="L33" s="122"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="38"/>
+      <c r="J33" s="211"/>
+      <c r="K33" s="210"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="37"/>
     </row>
     <row r="34" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A34" s="128"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="54"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="54"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="117"/>
-      <c r="J34" s="225"/>
-      <c r="K34" s="226"/>
-      <c r="L34" s="123"/>
-      <c r="M34" s="56"/>
-      <c r="N34" s="57"/>
+      <c r="A34" s="185"/>
+      <c r="B34" s="51"/>
+      <c r="C34" s="51"/>
+      <c r="D34" s="51"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="51"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="218"/>
+      <c r="J34" s="211"/>
+      <c r="K34" s="210"/>
+      <c r="L34" s="112"/>
+      <c r="M34" s="53"/>
+      <c r="N34" s="54"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="128"/>
-      <c r="B35" s="170" t="s">
+      <c r="A35" s="185"/>
+      <c r="B35" s="200" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="171"/>
-      <c r="D35" s="171"/>
-      <c r="E35" s="171"/>
-      <c r="F35" s="171"/>
-      <c r="G35" s="171"/>
-      <c r="H35" s="171"/>
-      <c r="I35" s="171"/>
-      <c r="J35" s="172"/>
-      <c r="K35" s="172"/>
-      <c r="L35" s="171"/>
-      <c r="M35" s="171"/>
-      <c r="N35" s="173"/>
+      <c r="C35" s="201"/>
+      <c r="D35" s="201"/>
+      <c r="E35" s="201"/>
+      <c r="F35" s="201"/>
+      <c r="G35" s="201"/>
+      <c r="H35" s="201"/>
+      <c r="I35" s="201"/>
+      <c r="J35" s="202"/>
+      <c r="K35" s="202"/>
+      <c r="L35" s="201"/>
+      <c r="M35" s="201"/>
+      <c r="N35" s="203"/>
     </row>
     <row r="36" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A36" s="128"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="59"/>
-      <c r="D36" s="58"/>
-      <c r="E36" s="174" t="s">
+      <c r="A36" s="185"/>
+      <c r="B36" s="55"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="55"/>
+      <c r="E36" s="204" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="175"/>
-      <c r="G36" s="176" t="s">
+      <c r="F36" s="205"/>
+      <c r="G36" s="131" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="177"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="61"/>
-      <c r="K36" s="62"/>
-      <c r="L36" s="63" t="s">
+      <c r="H36" s="206"/>
+      <c r="I36" s="57"/>
+      <c r="J36" s="58"/>
+      <c r="K36" s="59"/>
+      <c r="L36" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="M36" s="64" t="s">
+      <c r="M36" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="N36" s="65"/>
+      <c r="N36" s="62"/>
     </row>
     <row r="37" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A37" s="128"/>
-      <c r="B37" s="66" t="s">
+      <c r="A37" s="185"/>
+      <c r="B37" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="67"/>
-      <c r="D37" s="68" t="s">
+      <c r="C37" s="64"/>
+      <c r="D37" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="E37" s="178"/>
-      <c r="F37" s="179"/>
-      <c r="G37" s="178"/>
-      <c r="H37" s="179"/>
-      <c r="I37" s="69" t="s">
+      <c r="E37" s="153"/>
+      <c r="F37" s="154"/>
+      <c r="G37" s="153"/>
+      <c r="H37" s="154"/>
+      <c r="I37" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="J37" s="70" t="s">
+      <c r="J37" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="K37" s="71"/>
-      <c r="L37" s="72"/>
-      <c r="M37" s="72"/>
-      <c r="N37" s="73" t="s">
+      <c r="K37" s="68"/>
+      <c r="L37" s="69"/>
+      <c r="M37" s="69"/>
+      <c r="N37" s="70" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="128"/>
-      <c r="B38" s="74" t="s">
+      <c r="A38" s="185"/>
+      <c r="B38" s="71" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="75"/>
-      <c r="D38" s="76" t="s">
+      <c r="C38" s="72"/>
+      <c r="D38" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="180"/>
-      <c r="F38" s="181"/>
-      <c r="G38" s="180"/>
-      <c r="H38" s="181"/>
-      <c r="I38" s="77" t="s">
+      <c r="E38" s="115"/>
+      <c r="F38" s="116"/>
+      <c r="G38" s="115"/>
+      <c r="H38" s="116"/>
+      <c r="I38" s="74" t="s">
         <v>54</v>
       </c>
-      <c r="J38" s="78" t="s">
+      <c r="J38" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="K38" s="79"/>
-      <c r="L38" s="72"/>
-      <c r="M38" s="72"/>
-      <c r="N38" s="80" t="s">
+      <c r="K38" s="76"/>
+      <c r="L38" s="69"/>
+      <c r="M38" s="69"/>
+      <c r="N38" s="77" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="128"/>
-      <c r="B39" s="81" t="s">
+      <c r="A39" s="185"/>
+      <c r="B39" s="78" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="82"/>
-      <c r="D39" s="68" t="s">
+      <c r="C39" s="79"/>
+      <c r="D39" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="182"/>
-      <c r="F39" s="183"/>
-      <c r="G39" s="182"/>
-      <c r="H39" s="183"/>
-      <c r="I39" s="69" t="s">
+      <c r="E39" s="207"/>
+      <c r="F39" s="208"/>
+      <c r="G39" s="207"/>
+      <c r="H39" s="208"/>
+      <c r="I39" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="J39" s="78" t="s">
+      <c r="J39" s="75" t="s">
         <v>59</v>
       </c>
-      <c r="K39" s="79"/>
-      <c r="L39" s="72"/>
-      <c r="M39" s="72"/>
-      <c r="N39" s="38" t="s">
+      <c r="K39" s="76"/>
+      <c r="L39" s="69"/>
+      <c r="M39" s="69"/>
+      <c r="N39" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="128"/>
-      <c r="B40" s="74" t="s">
+      <c r="A40" s="185"/>
+      <c r="B40" s="71" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="75"/>
-      <c r="D40" s="83" t="s">
+      <c r="C40" s="72"/>
+      <c r="D40" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="184"/>
-      <c r="F40" s="185"/>
-      <c r="G40" s="186"/>
-      <c r="H40" s="187"/>
-      <c r="I40" s="84" t="s">
+      <c r="E40" s="144"/>
+      <c r="F40" s="145"/>
+      <c r="G40" s="146"/>
+      <c r="H40" s="147"/>
+      <c r="I40" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="J40" s="78" t="s">
+      <c r="J40" s="75" t="s">
         <v>62</v>
       </c>
-      <c r="K40" s="79"/>
-      <c r="L40" s="72"/>
-      <c r="M40" s="72"/>
-      <c r="N40" s="38" t="s">
+      <c r="K40" s="76"/>
+      <c r="L40" s="69"/>
+      <c r="M40" s="69"/>
+      <c r="N40" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A41" s="128"/>
-      <c r="B41" s="188" t="s">
+      <c r="A41" s="185"/>
+      <c r="B41" s="148" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="189"/>
-      <c r="D41" s="189"/>
-      <c r="E41" s="189"/>
-      <c r="F41" s="189"/>
-      <c r="G41" s="189"/>
-      <c r="H41" s="189"/>
-      <c r="I41" s="190"/>
-      <c r="J41" s="78" t="s">
+      <c r="C41" s="149"/>
+      <c r="D41" s="149"/>
+      <c r="E41" s="149"/>
+      <c r="F41" s="149"/>
+      <c r="G41" s="149"/>
+      <c r="H41" s="149"/>
+      <c r="I41" s="150"/>
+      <c r="J41" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="K41" s="79"/>
-      <c r="L41" s="72"/>
-      <c r="M41" s="72"/>
-      <c r="N41" s="38" t="s">
+      <c r="K41" s="76"/>
+      <c r="L41" s="69"/>
+      <c r="M41" s="69"/>
+      <c r="N41" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A42" s="128"/>
-      <c r="B42" s="191" t="s">
+      <c r="A42" s="185"/>
+      <c r="B42" s="151" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="192"/>
-      <c r="D42" s="85" t="s">
+      <c r="C42" s="152"/>
+      <c r="D42" s="82" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="178"/>
-      <c r="F42" s="179"/>
-      <c r="G42" s="193"/>
-      <c r="H42" s="194"/>
-      <c r="I42" s="69" t="s">
+      <c r="E42" s="153"/>
+      <c r="F42" s="154"/>
+      <c r="G42" s="155"/>
+      <c r="H42" s="156"/>
+      <c r="I42" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="J42" s="86" t="s">
+      <c r="J42" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="K42" s="87"/>
-      <c r="L42" s="72"/>
-      <c r="M42" s="72"/>
-      <c r="N42" s="88" t="s">
+      <c r="K42" s="84"/>
+      <c r="L42" s="69"/>
+      <c r="M42" s="69"/>
+      <c r="N42" s="85" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A43" s="128"/>
-      <c r="B43" s="89" t="s">
+      <c r="A43" s="185"/>
+      <c r="B43" s="86" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="90"/>
-      <c r="D43" s="91" t="s">
+      <c r="C43" s="87"/>
+      <c r="D43" s="88" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="180"/>
-      <c r="F43" s="181"/>
-      <c r="G43" s="195"/>
-      <c r="H43" s="196"/>
-      <c r="I43" s="92" t="s">
+      <c r="E43" s="115"/>
+      <c r="F43" s="116"/>
+      <c r="G43" s="117"/>
+      <c r="H43" s="118"/>
+      <c r="I43" s="89" t="s">
         <v>54</v>
       </c>
-      <c r="J43" s="176" t="s">
+      <c r="J43" s="131" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="209"/>
-      <c r="L43" s="209"/>
-      <c r="M43" s="209"/>
-      <c r="N43" s="210"/>
+      <c r="K43" s="132"/>
+      <c r="L43" s="132"/>
+      <c r="M43" s="132"/>
+      <c r="N43" s="133"/>
     </row>
     <row r="44" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A44" s="128"/>
-      <c r="B44" s="81" t="s">
+      <c r="A44" s="185"/>
+      <c r="B44" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="82"/>
-      <c r="D44" s="68" t="s">
+      <c r="C44" s="79"/>
+      <c r="D44" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="211"/>
-      <c r="F44" s="212"/>
-      <c r="G44" s="213"/>
-      <c r="H44" s="214"/>
-      <c r="I44" s="69" t="s">
+      <c r="E44" s="134"/>
+      <c r="F44" s="135"/>
+      <c r="G44" s="136"/>
+      <c r="H44" s="137"/>
+      <c r="I44" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="J44" s="70" t="s">
+      <c r="J44" s="67" t="s">
         <v>71</v>
       </c>
-      <c r="K44" s="71"/>
-      <c r="L44" s="93"/>
-      <c r="M44" s="93"/>
-      <c r="N44" s="73" t="s">
+      <c r="K44" s="68"/>
+      <c r="L44" s="90"/>
+      <c r="M44" s="90"/>
+      <c r="N44" s="70" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="128"/>
-      <c r="B45" s="74"/>
-      <c r="C45" s="75"/>
-      <c r="D45" s="91" t="s">
+      <c r="A45" s="185"/>
+      <c r="B45" s="71"/>
+      <c r="C45" s="72"/>
+      <c r="D45" s="88" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="215"/>
-      <c r="F45" s="216"/>
-      <c r="G45" s="217"/>
-      <c r="H45" s="218"/>
-      <c r="I45" s="92" t="s">
+      <c r="E45" s="138"/>
+      <c r="F45" s="139"/>
+      <c r="G45" s="140"/>
+      <c r="H45" s="141"/>
+      <c r="I45" s="89" t="s">
         <v>50</v>
       </c>
-      <c r="J45" s="78" t="s">
+      <c r="J45" s="75" t="s">
         <v>73</v>
       </c>
-      <c r="K45" s="79"/>
-      <c r="L45" s="94"/>
-      <c r="M45" s="72"/>
-      <c r="N45" s="38" t="s">
+      <c r="K45" s="76"/>
+      <c r="L45" s="91"/>
+      <c r="M45" s="69"/>
+      <c r="N45" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="128"/>
-      <c r="B46" s="81" t="s">
+      <c r="A46" s="185"/>
+      <c r="B46" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="82"/>
-      <c r="D46" s="68" t="s">
+      <c r="C46" s="79"/>
+      <c r="D46" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="E46" s="219"/>
-      <c r="F46" s="220"/>
-      <c r="G46" s="219"/>
-      <c r="H46" s="220"/>
-      <c r="I46" s="69" t="s">
+      <c r="E46" s="142"/>
+      <c r="F46" s="143"/>
+      <c r="G46" s="142"/>
+      <c r="H46" s="143"/>
+      <c r="I46" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="J46" s="86" t="s">
+      <c r="J46" s="83" t="s">
         <v>76</v>
       </c>
-      <c r="K46" s="87"/>
-      <c r="L46" s="95"/>
-      <c r="M46" s="72"/>
-      <c r="N46" s="88" t="s">
+      <c r="K46" s="84"/>
+      <c r="L46" s="92"/>
+      <c r="M46" s="69"/>
+      <c r="N46" s="85" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="128"/>
-      <c r="B47" s="74"/>
-      <c r="C47" s="75"/>
-      <c r="D47" s="91" t="s">
+      <c r="A47" s="185"/>
+      <c r="B47" s="71"/>
+      <c r="C47" s="72"/>
+      <c r="D47" s="88" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="197"/>
-      <c r="F47" s="198"/>
-      <c r="G47" s="198"/>
-      <c r="H47" s="199"/>
-      <c r="I47" s="91" t="s">
+      <c r="E47" s="119"/>
+      <c r="F47" s="120"/>
+      <c r="G47" s="120"/>
+      <c r="H47" s="121"/>
+      <c r="I47" s="88" t="s">
         <v>58</v>
       </c>
-      <c r="J47" s="200" t="s">
+      <c r="J47" s="122" t="s">
         <v>78</v>
       </c>
-      <c r="K47" s="201"/>
-      <c r="L47" s="201"/>
-      <c r="M47" s="201"/>
-      <c r="N47" s="202"/>
+      <c r="K47" s="123"/>
+      <c r="L47" s="123"/>
+      <c r="M47" s="123"/>
+      <c r="N47" s="124"/>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="129"/>
-      <c r="B48" s="96" t="s">
+      <c r="A48" s="186"/>
+      <c r="B48" s="93" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="97"/>
-      <c r="D48" s="98" t="s">
+      <c r="C48" s="94"/>
+      <c r="D48" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="203"/>
-      <c r="F48" s="204"/>
-      <c r="G48" s="204"/>
-      <c r="H48" s="205"/>
-      <c r="I48" s="99" t="s">
+      <c r="E48" s="125"/>
+      <c r="F48" s="126"/>
+      <c r="G48" s="126"/>
+      <c r="H48" s="127"/>
+      <c r="I48" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="206"/>
-      <c r="K48" s="207"/>
-      <c r="L48" s="207"/>
-      <c r="M48" s="207"/>
-      <c r="N48" s="208"/>
+      <c r="J48" s="128"/>
+      <c r="K48" s="129"/>
+      <c r="L48" s="129"/>
+      <c r="M48" s="129"/>
+      <c r="N48" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="71">
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="J47:N47"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="J48:N48"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="C2:N3"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:N7"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
     <mergeCell ref="A12:A48"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:N10"/>
@@ -3576,6 +3577,61 @@
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="G39:H39"/>
+    <mergeCell ref="C2:N3"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:N7"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="J47:N47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
->update upload daily log
</commit_message>
<xml_diff>
--- a/StarEnergi/App_Data/daily_log/DailyLogDay_BaseTemplate.xlsx
+++ b/StarEnergi/App_Data/daily_log/DailyLogDay_BaseTemplate.xlsx
@@ -427,7 +427,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="94">
+  <borders count="93">
     <border>
       <left/>
       <right/>
@@ -737,17 +737,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="hair">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1577,7 +1566,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="220">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1589,549 +1578,745 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="9" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="9" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="9" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="9" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="9" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="9" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="9" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="7" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="4" borderId="10" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="8" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="90" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="91" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="92" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="27" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="4" borderId="91" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="23" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="32" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="37" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="28" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="30" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="27" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="45" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="47" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="4" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="50" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="51" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="52" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="28" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="87" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="22" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="2" borderId="68" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="2" borderId="14" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="20" fontId="8" fillId="2" borderId="86" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="68" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="69" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="70" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="71" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="72" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="73" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="74" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="75" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="66" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="67" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="51" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="61" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="33" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="16" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="24" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="76" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="77" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="78" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="79" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="80" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="28" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="10" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="81" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="38" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="82" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="15" fontId="10" fillId="0" borderId="83" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="73" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="84" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="62" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="62" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="67" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="3" borderId="33" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="3" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="7" fillId="3" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="37" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="23" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="33" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="12" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="7" fillId="3" borderId="12" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="37" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="40" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="19" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="45" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="28" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="46" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="7" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="48" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="49" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="50" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="23" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="51" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="15" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="52" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="53" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="29" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="26" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="9" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="49" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="22" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="43" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="30" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="31" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="53" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="55" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="54" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="52" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="51" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="56" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="55" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="53" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="52" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="44" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="43" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="57" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="56" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="35" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="58" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="57" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="17" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="58" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="59" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="2" fontId="8" fillId="5" borderId="60" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="61" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="47" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="59" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="61" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="8" fillId="5" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="44" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="32" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="48" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="49" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="34" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="35" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="7" fillId="3" borderId="36" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="38" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="0" borderId="39" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="41" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="42" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="77" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="78" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="79" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="80" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="81" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="82" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="39" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="83" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="10" fillId="0" borderId="84" xfId="10" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="38" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="74" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="85" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="86" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="63" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="64" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="65" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="66" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="67" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="68" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="2" borderId="69" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="2" borderId="14" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="8" fillId="2" borderId="87" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="69" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="70" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="71" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="72" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="73" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="74" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="75" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="76" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="67" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="68" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="52" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="56" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="31" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="62" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="34" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="36" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="60" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="8" fillId="5" borderId="61" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="59" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="40" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="89" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="91" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="92" xfId="11" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="5" borderId="93" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="7" fillId="4" borderId="92" xfId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="88" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="39" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="58" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -2210,7 +2395,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
+      <xdr:colOff>609600</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -2231,7 +2416,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="38100" y="38100"/>
-          <a:ext cx="1181100" cy="695325"/>
+          <a:ext cx="1186016" cy="699319"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2537,15 +2722,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="93" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="93" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="97"/>
+    <col min="1" max="1" width="9.140625" style="7"/>
     <col min="2" max="2" width="9.140625" style="6"/>
-    <col min="3" max="3" width="9.140625" style="98"/>
+    <col min="3" max="3" width="9.140625" style="8"/>
     <col min="4" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
@@ -2566,1001 +2751,1056 @@
       <c r="N1" s="5"/>
     </row>
     <row r="2" spans="1:14">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="157" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="157"/>
-      <c r="E2" s="157"/>
-      <c r="F2" s="157"/>
-      <c r="G2" s="157"/>
-      <c r="H2" s="157"/>
-      <c r="I2" s="157"/>
-      <c r="J2" s="157"/>
-      <c r="K2" s="157"/>
-      <c r="L2" s="157"/>
-      <c r="M2" s="157"/>
-      <c r="N2" s="158"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="139"/>
     </row>
     <row r="3" spans="1:14">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="157"/>
-      <c r="D3" s="157"/>
-      <c r="E3" s="157"/>
-      <c r="F3" s="157"/>
-      <c r="G3" s="157"/>
-      <c r="H3" s="157"/>
-      <c r="I3" s="157"/>
-      <c r="J3" s="157"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="157"/>
-      <c r="M3" s="157"/>
-      <c r="N3" s="158"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="139"/>
     </row>
     <row r="4" spans="1:14" ht="19.5">
-      <c r="A4" s="9"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="13"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="15"/>
     </row>
     <row r="5" spans="1:14" ht="14.25">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="N5" s="16"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="18"/>
     </row>
     <row r="6" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="16"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="18"/>
     </row>
     <row r="7" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A7" s="159" t="s">
+      <c r="A7" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="160"/>
-      <c r="C7" s="161"/>
-      <c r="D7" s="18" t="s">
+      <c r="B7" s="141"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="162" t="s">
+      <c r="E7" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="161"/>
-      <c r="G7" s="162" t="s">
+      <c r="F7" s="142"/>
+      <c r="G7" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="160"/>
-      <c r="K7" s="160"/>
-      <c r="L7" s="160"/>
-      <c r="M7" s="160"/>
-      <c r="N7" s="163"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="144"/>
     </row>
     <row r="8" spans="1:14" ht="13.5" customHeight="1" thickTop="1">
-      <c r="A8" s="164">
+      <c r="A8" s="145">
         <v>41459</v>
       </c>
-      <c r="B8" s="165"/>
-      <c r="C8" s="166"/>
-      <c r="D8" s="170"/>
-      <c r="E8" s="172"/>
-      <c r="F8" s="173"/>
-      <c r="G8" s="176"/>
-      <c r="H8" s="177"/>
-      <c r="I8" s="176"/>
-      <c r="J8" s="177"/>
-      <c r="K8" s="176"/>
-      <c r="L8" s="177"/>
-      <c r="M8" s="178"/>
-      <c r="N8" s="179"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="153"/>
+      <c r="F8" s="154"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="158"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="157"/>
+      <c r="L8" s="158"/>
+      <c r="M8" s="159"/>
+      <c r="N8" s="160"/>
     </row>
     <row r="9" spans="1:14" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A9" s="167"/>
-      <c r="B9" s="168"/>
-      <c r="C9" s="169"/>
-      <c r="D9" s="171"/>
-      <c r="E9" s="174"/>
-      <c r="F9" s="175"/>
-      <c r="G9" s="180"/>
-      <c r="H9" s="181"/>
-      <c r="I9" s="180"/>
-      <c r="J9" s="181"/>
-      <c r="K9" s="180"/>
-      <c r="L9" s="181"/>
-      <c r="M9" s="182"/>
-      <c r="N9" s="183"/>
+      <c r="A9" s="148"/>
+      <c r="B9" s="149"/>
+      <c r="C9" s="150"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="155"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="161"/>
+      <c r="H9" s="162"/>
+      <c r="I9" s="161"/>
+      <c r="J9" s="162"/>
+      <c r="K9" s="161"/>
+      <c r="L9" s="162"/>
+      <c r="M9" s="163"/>
+      <c r="N9" s="164"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="187" t="s">
+      <c r="A10" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="189" t="s">
+      <c r="B10" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="190"/>
-      <c r="D10" s="190"/>
-      <c r="E10" s="190"/>
-      <c r="F10" s="190"/>
-      <c r="G10" s="190"/>
-      <c r="H10" s="190"/>
-      <c r="I10" s="190"/>
-      <c r="J10" s="190"/>
-      <c r="K10" s="190"/>
-      <c r="L10" s="190"/>
-      <c r="M10" s="190"/>
-      <c r="N10" s="191"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="114"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="114"/>
+      <c r="K10" s="114"/>
+      <c r="L10" s="114"/>
+      <c r="M10" s="114"/>
+      <c r="N10" s="115"/>
     </row>
     <row r="11" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A11" s="188"/>
-      <c r="B11" s="192" t="s">
+      <c r="A11" s="112"/>
+      <c r="B11" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="193"/>
-      <c r="D11" s="193"/>
-      <c r="E11" s="193"/>
-      <c r="F11" s="193"/>
-      <c r="G11" s="193"/>
-      <c r="H11" s="193"/>
-      <c r="I11" s="193"/>
-      <c r="J11" s="194" t="s">
+      <c r="C11" s="117"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="195"/>
-      <c r="L11" s="195"/>
-      <c r="M11" s="195"/>
-      <c r="N11" s="196"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="120"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="184">
+      <c r="A12" s="108">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B12" s="197" t="s">
+      <c r="B12" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="D12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="197" t="s">
+      <c r="F12" s="121" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="20" t="s">
+      <c r="H12" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="21" t="s">
+      <c r="I12" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="J12" s="22"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="20" t="s">
+      <c r="J12" s="24"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="M12" s="20" t="s">
+      <c r="M12" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="N12" s="24"/>
+      <c r="N12" s="26"/>
     </row>
     <row r="13" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A13" s="185"/>
-      <c r="B13" s="198"/>
-      <c r="C13" s="25" t="s">
+      <c r="A13" s="109"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="26" t="s">
+      <c r="E13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="199"/>
-      <c r="G13" s="26" t="s">
+      <c r="F13" s="123"/>
+      <c r="G13" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="26" t="s">
+      <c r="H13" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="22"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="28" t="s">
+      <c r="J13" s="24"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="28" t="s">
+      <c r="M13" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="N13" s="29"/>
+      <c r="N13" s="31"/>
     </row>
     <row r="14" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A14" s="185"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="31"/>
-      <c r="F14" s="30"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="212"/>
-      <c r="J14" s="213"/>
-      <c r="K14" s="214"/>
-      <c r="L14" s="107"/>
-      <c r="M14" s="32"/>
+      <c r="A14" s="109"/>
+      <c r="B14" s="102"/>
+      <c r="C14" s="95"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="99"/>
+      <c r="J14" s="202"/>
+      <c r="K14" s="203"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="33"/>
       <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
-      <c r="A15" s="185"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="31"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="31"/>
-      <c r="I15" s="215"/>
-      <c r="J15" s="211"/>
-      <c r="K15" s="210"/>
-      <c r="L15" s="108"/>
-      <c r="M15" s="31"/>
+      <c r="A15" s="109"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="103"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="100"/>
+      <c r="J15" s="204"/>
+      <c r="K15" s="205"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="36"/>
       <c r="N15" s="37"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1">
-      <c r="A16" s="185"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="215"/>
-      <c r="J16" s="209"/>
-      <c r="K16" s="210"/>
-      <c r="L16" s="109"/>
-      <c r="M16" s="31"/>
+      <c r="A16" s="109"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="100"/>
+      <c r="J16" s="206"/>
+      <c r="K16" s="205"/>
+      <c r="L16" s="35"/>
+      <c r="M16" s="36"/>
       <c r="N16" s="37"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="185"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="35"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="215"/>
-      <c r="J17" s="209"/>
-      <c r="K17" s="210"/>
-      <c r="L17" s="109"/>
-      <c r="M17" s="31"/>
+      <c r="A17" s="109"/>
+      <c r="B17" s="103"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="100"/>
+      <c r="J17" s="206"/>
+      <c r="K17" s="205"/>
+      <c r="L17" s="35"/>
+      <c r="M17" s="36"/>
       <c r="N17" s="37"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="185"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="215"/>
-      <c r="J18" s="209"/>
-      <c r="K18" s="210"/>
-      <c r="L18" s="110"/>
-      <c r="M18" s="38"/>
+      <c r="A18" s="109"/>
+      <c r="B18" s="103"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="96"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="100"/>
+      <c r="J18" s="206"/>
+      <c r="K18" s="205"/>
+      <c r="L18" s="35"/>
+      <c r="M18" s="36"/>
       <c r="N18" s="37"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="185"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="35"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="215"/>
-      <c r="J19" s="209"/>
-      <c r="K19" s="210"/>
-      <c r="L19" s="109"/>
-      <c r="M19" s="31"/>
+      <c r="A19" s="109"/>
+      <c r="B19" s="103"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="96"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="100"/>
+      <c r="J19" s="206"/>
+      <c r="K19" s="205"/>
+      <c r="L19" s="35"/>
+      <c r="M19" s="36"/>
       <c r="N19" s="37"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="185"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="215"/>
-      <c r="J20" s="209"/>
-      <c r="K20" s="210"/>
-      <c r="L20" s="109"/>
-      <c r="M20" s="31"/>
+      <c r="A20" s="109"/>
+      <c r="B20" s="103"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="105"/>
+      <c r="G20" s="96"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="206"/>
+      <c r="K20" s="205"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="36"/>
       <c r="N20" s="37"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="185"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="215"/>
-      <c r="J21" s="209"/>
-      <c r="K21" s="210"/>
-      <c r="L21" s="109"/>
-      <c r="M21" s="31"/>
+      <c r="A21" s="109"/>
+      <c r="B21" s="103"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="95"/>
+      <c r="E21" s="95"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="96"/>
+      <c r="H21" s="95"/>
+      <c r="I21" s="100"/>
+      <c r="J21" s="206"/>
+      <c r="K21" s="205"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="36"/>
       <c r="N21" s="37"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="185"/>
-      <c r="B22" s="35"/>
-      <c r="C22" s="103"/>
-      <c r="D22" s="103"/>
-      <c r="E22" s="103"/>
-      <c r="F22" s="40"/>
-      <c r="G22" s="36"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="215"/>
-      <c r="J22" s="209"/>
-      <c r="K22" s="210"/>
-      <c r="L22" s="109"/>
-      <c r="M22" s="31"/>
+      <c r="A22" s="109"/>
+      <c r="B22" s="103"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="95"/>
+      <c r="E22" s="95"/>
+      <c r="F22" s="106"/>
+      <c r="G22" s="96"/>
+      <c r="H22" s="95"/>
+      <c r="I22" s="100"/>
+      <c r="J22" s="206"/>
+      <c r="K22" s="205"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="36"/>
       <c r="N22" s="37"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="185"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="40"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="215"/>
-      <c r="J23" s="209"/>
-      <c r="K23" s="210"/>
-      <c r="L23" s="109"/>
-      <c r="M23" s="31"/>
+      <c r="A23" s="109"/>
+      <c r="B23" s="103"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="95"/>
+      <c r="E23" s="95"/>
+      <c r="F23" s="106"/>
+      <c r="G23" s="96"/>
+      <c r="H23" s="95"/>
+      <c r="I23" s="100"/>
+      <c r="J23" s="206"/>
+      <c r="K23" s="205"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="36"/>
       <c r="N23" s="37"/>
     </row>
-    <row r="24" spans="1:14" ht="15">
-      <c r="A24" s="185"/>
-      <c r="B24" s="35"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="104"/>
-      <c r="H24" s="105"/>
-      <c r="I24" s="215"/>
-      <c r="J24" s="209"/>
-      <c r="K24" s="210"/>
-      <c r="L24" s="109"/>
-      <c r="M24" s="31"/>
+    <row r="24" spans="1:14">
+      <c r="A24" s="109"/>
+      <c r="B24" s="103"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
+      <c r="F24" s="105"/>
+      <c r="G24" s="96"/>
+      <c r="H24" s="95"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="206"/>
+      <c r="K24" s="205"/>
+      <c r="L24" s="35"/>
+      <c r="M24" s="36"/>
       <c r="N24" s="37"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="185"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="43"/>
-      <c r="D25" s="31"/>
-      <c r="E25" s="43"/>
-      <c r="F25" s="35"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="106"/>
-      <c r="I25" s="215"/>
-      <c r="J25" s="209"/>
-      <c r="K25" s="210"/>
-      <c r="L25" s="109"/>
-      <c r="M25" s="31"/>
+      <c r="A25" s="109"/>
+      <c r="B25" s="103"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="95"/>
+      <c r="E25" s="95"/>
+      <c r="F25" s="103"/>
+      <c r="G25" s="96"/>
+      <c r="H25" s="95"/>
+      <c r="I25" s="100"/>
+      <c r="J25" s="206"/>
+      <c r="K25" s="205"/>
+      <c r="L25" s="35"/>
+      <c r="M25" s="36"/>
       <c r="N25" s="37"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="185"/>
-      <c r="B26" s="35"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="43"/>
-      <c r="F26" s="35"/>
-      <c r="G26" s="99"/>
-      <c r="H26" s="100"/>
-      <c r="I26" s="215"/>
-      <c r="J26" s="209"/>
-      <c r="K26" s="210"/>
-      <c r="L26" s="109"/>
-      <c r="M26" s="31"/>
+      <c r="A26" s="109"/>
+      <c r="B26" s="103"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="103"/>
+      <c r="G26" s="96"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="100"/>
+      <c r="J26" s="206"/>
+      <c r="K26" s="205"/>
+      <c r="L26" s="35"/>
+      <c r="M26" s="36"/>
       <c r="N26" s="37"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="185"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="31"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="99"/>
-      <c r="H27" s="100"/>
-      <c r="I27" s="215"/>
-      <c r="J27" s="209"/>
-      <c r="K27" s="210"/>
-      <c r="L27" s="109"/>
-      <c r="M27" s="31"/>
+      <c r="A27" s="109"/>
+      <c r="B27" s="104"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="103"/>
+      <c r="G27" s="96"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="100"/>
+      <c r="J27" s="206"/>
+      <c r="K27" s="205"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="36"/>
       <c r="N27" s="37"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="185"/>
-      <c r="B28" s="35"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="113"/>
-      <c r="G28" s="114"/>
-      <c r="H28" s="114"/>
-      <c r="I28" s="215"/>
-      <c r="J28" s="209"/>
-      <c r="K28" s="210"/>
-      <c r="L28" s="109"/>
-      <c r="M28" s="31"/>
+      <c r="A28" s="109"/>
+      <c r="B28" s="103"/>
+      <c r="C28" s="96"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="98"/>
+      <c r="F28" s="107"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="101"/>
+      <c r="I28" s="100"/>
+      <c r="J28" s="206"/>
+      <c r="K28" s="205"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="36"/>
       <c r="N28" s="37"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="185"/>
-      <c r="B29" s="45" t="s">
+      <c r="A29" s="109"/>
+      <c r="B29" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="D29" s="45" t="s">
+      <c r="D29" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="45" t="s">
+      <c r="E29" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="F29" s="45" t="s">
+      <c r="F29" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="45" t="s">
+      <c r="G29" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="H29" s="45" t="s">
+      <c r="H29" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="I29" s="216" t="s">
+      <c r="I29" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="211"/>
-      <c r="K29" s="210"/>
-      <c r="L29" s="109"/>
-      <c r="M29" s="31"/>
+      <c r="J29" s="204"/>
+      <c r="K29" s="205"/>
+      <c r="L29" s="35"/>
+      <c r="M29" s="36"/>
       <c r="N29" s="37"/>
     </row>
     <row r="30" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A30" s="185"/>
-      <c r="B30" s="46" t="s">
+      <c r="A30" s="109"/>
+      <c r="B30" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="C30" s="46" t="s">
+      <c r="C30" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D30" s="46" t="s">
+      <c r="D30" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="46" t="s">
+      <c r="E30" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="F30" s="46" t="s">
+      <c r="F30" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="G30" s="46" t="s">
+      <c r="G30" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="H30" s="46" t="s">
+      <c r="H30" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="I30" s="217" t="s">
+      <c r="I30" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="211"/>
-      <c r="K30" s="210"/>
-      <c r="L30" s="109"/>
-      <c r="M30" s="31"/>
+      <c r="J30" s="204"/>
+      <c r="K30" s="205"/>
+      <c r="L30" s="35"/>
+      <c r="M30" s="36"/>
       <c r="N30" s="37"/>
     </row>
     <row r="31" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A31" s="185"/>
-      <c r="B31" s="47"/>
-      <c r="C31" s="47"/>
-      <c r="D31" s="47"/>
-      <c r="E31" s="47"/>
-      <c r="F31" s="47"/>
-      <c r="G31" s="47"/>
-      <c r="H31" s="47"/>
-      <c r="I31" s="218"/>
-      <c r="J31" s="211"/>
-      <c r="K31" s="210"/>
-      <c r="L31" s="111"/>
-      <c r="M31" s="43"/>
+      <c r="A31" s="109"/>
+      <c r="B31" s="42"/>
+      <c r="C31" s="42"/>
+      <c r="D31" s="42"/>
+      <c r="E31" s="42"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="42"/>
+      <c r="H31" s="42"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="204"/>
+      <c r="K31" s="205"/>
+      <c r="L31" s="35"/>
+      <c r="M31" s="36"/>
       <c r="N31" s="37"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="185"/>
-      <c r="B32" s="48" t="s">
+      <c r="A32" s="109"/>
+      <c r="B32" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="45" t="s">
+      <c r="D32" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="E32" s="45" t="s">
+      <c r="E32" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="F32" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="G32" s="45" t="s">
+      <c r="G32" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="H32" s="45" t="s">
+      <c r="H32" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="I32" s="216" t="s">
+      <c r="I32" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="J32" s="211"/>
-      <c r="K32" s="210"/>
-      <c r="L32" s="109"/>
-      <c r="M32" s="31"/>
+      <c r="J32" s="204"/>
+      <c r="K32" s="205"/>
+      <c r="L32" s="35"/>
+      <c r="M32" s="36"/>
       <c r="N32" s="37"/>
     </row>
     <row r="33" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A33" s="185"/>
-      <c r="B33" s="46" t="s">
+      <c r="A33" s="109"/>
+      <c r="B33" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="46" t="s">
+      <c r="C33" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="D33" s="46" t="s">
+      <c r="D33" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="46" t="s">
+      <c r="E33" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="F33" s="46" t="s">
+      <c r="F33" s="40" t="s">
         <v>45</v>
       </c>
-      <c r="G33" s="46" t="s">
+      <c r="G33" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="H33" s="50" t="s">
+      <c r="H33" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="I33" s="219" t="s">
+      <c r="I33" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="J33" s="211"/>
-      <c r="K33" s="210"/>
-      <c r="L33" s="111"/>
-      <c r="M33" s="43"/>
+      <c r="J33" s="204"/>
+      <c r="K33" s="205"/>
+      <c r="L33" s="35"/>
+      <c r="M33" s="36"/>
       <c r="N33" s="37"/>
     </row>
     <row r="34" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A34" s="185"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="218"/>
-      <c r="J34" s="211"/>
-      <c r="K34" s="210"/>
-      <c r="L34" s="112"/>
-      <c r="M34" s="53"/>
-      <c r="N34" s="54"/>
+      <c r="A34" s="109"/>
+      <c r="B34" s="48"/>
+      <c r="C34" s="48"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
+      <c r="F34" s="48"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="204"/>
+      <c r="K34" s="205"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="51"/>
+      <c r="N34" s="52"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="185"/>
-      <c r="B35" s="200" t="s">
+      <c r="A35" s="109"/>
+      <c r="B35" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="201"/>
-      <c r="D35" s="201"/>
-      <c r="E35" s="201"/>
-      <c r="F35" s="201"/>
-      <c r="G35" s="201"/>
-      <c r="H35" s="201"/>
-      <c r="I35" s="201"/>
-      <c r="J35" s="202"/>
-      <c r="K35" s="202"/>
-      <c r="L35" s="201"/>
-      <c r="M35" s="201"/>
-      <c r="N35" s="203"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="125"/>
+      <c r="E35" s="125"/>
+      <c r="F35" s="125"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="125"/>
+      <c r="I35" s="125"/>
+      <c r="J35" s="126"/>
+      <c r="K35" s="126"/>
+      <c r="L35" s="125"/>
+      <c r="M35" s="125"/>
+      <c r="N35" s="127"/>
     </row>
     <row r="36" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A36" s="185"/>
-      <c r="B36" s="55"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="204" t="s">
+      <c r="A36" s="109"/>
+      <c r="B36" s="53"/>
+      <c r="C36" s="54"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="205"/>
-      <c r="G36" s="131" t="s">
+      <c r="F36" s="129"/>
+      <c r="G36" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="206"/>
-      <c r="I36" s="57"/>
-      <c r="J36" s="58"/>
-      <c r="K36" s="59"/>
-      <c r="L36" s="60" t="s">
+      <c r="H36" s="131"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="56"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="M36" s="61" t="s">
+      <c r="M36" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="N36" s="62"/>
+      <c r="N36" s="60"/>
     </row>
     <row r="37" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A37" s="185"/>
-      <c r="B37" s="63" t="s">
+      <c r="A37" s="109"/>
+      <c r="B37" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C37" s="64"/>
-      <c r="D37" s="65" t="s">
+      <c r="C37" s="62"/>
+      <c r="D37" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="E37" s="153"/>
-      <c r="F37" s="154"/>
-      <c r="G37" s="153"/>
-      <c r="H37" s="154"/>
-      <c r="I37" s="66" t="s">
+      <c r="E37" s="132"/>
+      <c r="F37" s="133"/>
+      <c r="G37" s="132"/>
+      <c r="H37" s="133"/>
+      <c r="I37" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="J37" s="67" t="s">
+      <c r="J37" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="K37" s="68"/>
-      <c r="L37" s="69"/>
-      <c r="M37" s="69"/>
-      <c r="N37" s="70" t="s">
+      <c r="K37" s="66"/>
+      <c r="L37" s="67"/>
+      <c r="M37" s="67"/>
+      <c r="N37" s="68" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="185"/>
-      <c r="B38" s="71" t="s">
+      <c r="A38" s="109"/>
+      <c r="B38" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="72"/>
-      <c r="D38" s="73" t="s">
+      <c r="C38" s="70"/>
+      <c r="D38" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="115"/>
-      <c r="F38" s="116"/>
-      <c r="G38" s="115"/>
-      <c r="H38" s="116"/>
-      <c r="I38" s="74" t="s">
+      <c r="E38" s="134"/>
+      <c r="F38" s="135"/>
+      <c r="G38" s="134"/>
+      <c r="H38" s="135"/>
+      <c r="I38" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="J38" s="75" t="s">
+      <c r="J38" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="K38" s="76"/>
-      <c r="L38" s="69"/>
-      <c r="M38" s="69"/>
-      <c r="N38" s="77" t="s">
+      <c r="K38" s="74"/>
+      <c r="L38" s="67"/>
+      <c r="M38" s="67"/>
+      <c r="N38" s="75" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="185"/>
-      <c r="B39" s="78" t="s">
+      <c r="A39" s="109"/>
+      <c r="B39" s="76" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="79"/>
-      <c r="D39" s="65" t="s">
+      <c r="C39" s="77"/>
+      <c r="D39" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="207"/>
-      <c r="F39" s="208"/>
-      <c r="G39" s="207"/>
-      <c r="H39" s="208"/>
-      <c r="I39" s="66" t="s">
+      <c r="E39" s="136"/>
+      <c r="F39" s="137"/>
+      <c r="G39" s="136"/>
+      <c r="H39" s="137"/>
+      <c r="I39" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="J39" s="75" t="s">
+      <c r="J39" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="K39" s="76"/>
-      <c r="L39" s="69"/>
-      <c r="M39" s="69"/>
+      <c r="K39" s="74"/>
+      <c r="L39" s="67"/>
+      <c r="M39" s="67"/>
       <c r="N39" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="185"/>
-      <c r="B40" s="71" t="s">
+      <c r="A40" s="109"/>
+      <c r="B40" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="C40" s="72"/>
-      <c r="D40" s="80" t="s">
+      <c r="C40" s="70"/>
+      <c r="D40" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="144"/>
-      <c r="F40" s="145"/>
-      <c r="G40" s="146"/>
-      <c r="H40" s="147"/>
-      <c r="I40" s="81" t="s">
+      <c r="E40" s="165"/>
+      <c r="F40" s="166"/>
+      <c r="G40" s="167"/>
+      <c r="H40" s="168"/>
+      <c r="I40" s="79" t="s">
         <v>58</v>
       </c>
-      <c r="J40" s="75" t="s">
+      <c r="J40" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="K40" s="76"/>
-      <c r="L40" s="69"/>
-      <c r="M40" s="69"/>
+      <c r="K40" s="74"/>
+      <c r="L40" s="67"/>
+      <c r="M40" s="67"/>
       <c r="N40" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A41" s="185"/>
-      <c r="B41" s="148" t="s">
+      <c r="A41" s="109"/>
+      <c r="B41" s="169" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="149"/>
-      <c r="D41" s="149"/>
-      <c r="E41" s="149"/>
-      <c r="F41" s="149"/>
-      <c r="G41" s="149"/>
-      <c r="H41" s="149"/>
-      <c r="I41" s="150"/>
-      <c r="J41" s="75" t="s">
+      <c r="C41" s="170"/>
+      <c r="D41" s="170"/>
+      <c r="E41" s="170"/>
+      <c r="F41" s="170"/>
+      <c r="G41" s="170"/>
+      <c r="H41" s="170"/>
+      <c r="I41" s="171"/>
+      <c r="J41" s="73" t="s">
         <v>64</v>
       </c>
-      <c r="K41" s="76"/>
-      <c r="L41" s="69"/>
-      <c r="M41" s="69"/>
+      <c r="K41" s="74"/>
+      <c r="L41" s="67"/>
+      <c r="M41" s="67"/>
       <c r="N41" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A42" s="185"/>
-      <c r="B42" s="151" t="s">
+      <c r="A42" s="109"/>
+      <c r="B42" s="172" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="152"/>
-      <c r="D42" s="82" t="s">
+      <c r="C42" s="173"/>
+      <c r="D42" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="153"/>
-      <c r="F42" s="154"/>
-      <c r="G42" s="155"/>
-      <c r="H42" s="156"/>
-      <c r="I42" s="66" t="s">
+      <c r="E42" s="132"/>
+      <c r="F42" s="133"/>
+      <c r="G42" s="174"/>
+      <c r="H42" s="175"/>
+      <c r="I42" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="J42" s="83" t="s">
+      <c r="J42" s="81" t="s">
         <v>66</v>
       </c>
-      <c r="K42" s="84"/>
-      <c r="L42" s="69"/>
-      <c r="M42" s="69"/>
-      <c r="N42" s="85" t="s">
+      <c r="K42" s="82"/>
+      <c r="L42" s="67"/>
+      <c r="M42" s="67"/>
+      <c r="N42" s="83" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A43" s="185"/>
-      <c r="B43" s="86" t="s">
+      <c r="A43" s="109"/>
+      <c r="B43" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="C43" s="87"/>
-      <c r="D43" s="88" t="s">
+      <c r="C43" s="85"/>
+      <c r="D43" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="115"/>
-      <c r="F43" s="116"/>
-      <c r="G43" s="117"/>
-      <c r="H43" s="118"/>
-      <c r="I43" s="89" t="s">
+      <c r="E43" s="134"/>
+      <c r="F43" s="135"/>
+      <c r="G43" s="176"/>
+      <c r="H43" s="177"/>
+      <c r="I43" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="J43" s="131" t="s">
+      <c r="J43" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="132"/>
-      <c r="L43" s="132"/>
-      <c r="M43" s="132"/>
-      <c r="N43" s="133"/>
+      <c r="K43" s="190"/>
+      <c r="L43" s="190"/>
+      <c r="M43" s="190"/>
+      <c r="N43" s="191"/>
     </row>
     <row r="44" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A44" s="185"/>
-      <c r="B44" s="78" t="s">
+      <c r="A44" s="109"/>
+      <c r="B44" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="C44" s="79"/>
-      <c r="D44" s="65" t="s">
+      <c r="C44" s="77"/>
+      <c r="D44" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="134"/>
-      <c r="F44" s="135"/>
-      <c r="G44" s="136"/>
-      <c r="H44" s="137"/>
-      <c r="I44" s="66" t="s">
+      <c r="E44" s="192"/>
+      <c r="F44" s="193"/>
+      <c r="G44" s="194"/>
+      <c r="H44" s="195"/>
+      <c r="I44" s="64" t="s">
         <v>50</v>
       </c>
-      <c r="J44" s="67" t="s">
+      <c r="J44" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="K44" s="68"/>
-      <c r="L44" s="90"/>
-      <c r="M44" s="90"/>
-      <c r="N44" s="70" t="s">
+      <c r="K44" s="66"/>
+      <c r="L44" s="88"/>
+      <c r="M44" s="88"/>
+      <c r="N44" s="68" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="185"/>
-      <c r="B45" s="71"/>
-      <c r="C45" s="72"/>
-      <c r="D45" s="88" t="s">
+      <c r="A45" s="109"/>
+      <c r="B45" s="69"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="138"/>
-      <c r="F45" s="139"/>
-      <c r="G45" s="140"/>
-      <c r="H45" s="141"/>
-      <c r="I45" s="89" t="s">
+      <c r="E45" s="196"/>
+      <c r="F45" s="197"/>
+      <c r="G45" s="198"/>
+      <c r="H45" s="199"/>
+      <c r="I45" s="87" t="s">
         <v>50</v>
       </c>
-      <c r="J45" s="75" t="s">
+      <c r="J45" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="K45" s="76"/>
-      <c r="L45" s="91"/>
-      <c r="M45" s="69"/>
+      <c r="K45" s="74"/>
+      <c r="L45" s="89"/>
+      <c r="M45" s="67"/>
       <c r="N45" s="37" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="185"/>
-      <c r="B46" s="78" t="s">
+      <c r="A46" s="109"/>
+      <c r="B46" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="C46" s="79"/>
-      <c r="D46" s="65" t="s">
+      <c r="C46" s="77"/>
+      <c r="D46" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="E46" s="142"/>
-      <c r="F46" s="143"/>
-      <c r="G46" s="142"/>
-      <c r="H46" s="143"/>
-      <c r="I46" s="66" t="s">
+      <c r="E46" s="200"/>
+      <c r="F46" s="201"/>
+      <c r="G46" s="200"/>
+      <c r="H46" s="201"/>
+      <c r="I46" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="J46" s="83" t="s">
+      <c r="J46" s="81" t="s">
         <v>76</v>
       </c>
-      <c r="K46" s="84"/>
-      <c r="L46" s="92"/>
-      <c r="M46" s="69"/>
-      <c r="N46" s="85" t="s">
+      <c r="K46" s="82"/>
+      <c r="L46" s="90"/>
+      <c r="M46" s="67"/>
+      <c r="N46" s="83" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="185"/>
-      <c r="B47" s="71"/>
-      <c r="C47" s="72"/>
-      <c r="D47" s="88" t="s">
+      <c r="A47" s="109"/>
+      <c r="B47" s="69"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="119"/>
-      <c r="F47" s="120"/>
-      <c r="G47" s="120"/>
-      <c r="H47" s="121"/>
-      <c r="I47" s="88" t="s">
+      <c r="E47" s="178"/>
+      <c r="F47" s="179"/>
+      <c r="G47" s="179"/>
+      <c r="H47" s="180"/>
+      <c r="I47" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="J47" s="122" t="s">
+      <c r="J47" s="181" t="s">
         <v>78</v>
       </c>
-      <c r="K47" s="123"/>
-      <c r="L47" s="123"/>
-      <c r="M47" s="123"/>
-      <c r="N47" s="124"/>
+      <c r="K47" s="182"/>
+      <c r="L47" s="182"/>
+      <c r="M47" s="182"/>
+      <c r="N47" s="183"/>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="186"/>
-      <c r="B48" s="93" t="s">
+      <c r="A48" s="110"/>
+      <c r="B48" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="C48" s="94"/>
-      <c r="D48" s="95" t="s">
+      <c r="C48" s="92"/>
+      <c r="D48" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="125"/>
-      <c r="F48" s="126"/>
-      <c r="G48" s="126"/>
-      <c r="H48" s="127"/>
-      <c r="I48" s="96" t="s">
+      <c r="E48" s="184"/>
+      <c r="F48" s="185"/>
+      <c r="G48" s="185"/>
+      <c r="H48" s="186"/>
+      <c r="I48" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="128"/>
-      <c r="K48" s="129"/>
-      <c r="L48" s="129"/>
-      <c r="M48" s="129"/>
-      <c r="N48" s="130"/>
+      <c r="J48" s="187"/>
+      <c r="K48" s="188"/>
+      <c r="L48" s="188"/>
+      <c r="M48" s="188"/>
+      <c r="N48" s="189"/>
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="E47:H47"/>
+    <mergeCell ref="J47:N47"/>
+    <mergeCell ref="E48:H48"/>
+    <mergeCell ref="J48:N48"/>
+    <mergeCell ref="J43:N43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="C2:N3"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:N7"/>
+    <mergeCell ref="A8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="E8:F9"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="K9:L9"/>
+    <mergeCell ref="M9:N9"/>
     <mergeCell ref="A12:A48"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="B10:N10"/>
@@ -3577,61 +3817,6 @@
     <mergeCell ref="G38:H38"/>
     <mergeCell ref="E39:F39"/>
     <mergeCell ref="G39:H39"/>
-    <mergeCell ref="C2:N3"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:N7"/>
-    <mergeCell ref="A8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="E8:F9"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="K9:L9"/>
-    <mergeCell ref="M9:N9"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="G40:H40"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="E47:H47"/>
-    <mergeCell ref="J47:N47"/>
-    <mergeCell ref="E48:H48"/>
-    <mergeCell ref="J48:N48"/>
-    <mergeCell ref="J43:N43"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="J33:K33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
->add workflow to incident controller
</commit_message>
<xml_diff>
--- a/StarEnergi/App_Data/daily_log/DailyLogDay_BaseTemplate.xlsx
+++ b/StarEnergi/App_Data/daily_log/DailyLogDay_BaseTemplate.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="FormFracas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -1923,6 +1923,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="8" fillId="6" borderId="22" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="20" fontId="8" fillId="2" borderId="68" xfId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
@@ -2312,10 +2316,6 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="8" fillId="6" borderId="22" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -2370,53 +2370,7 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="38100" y="38100"/>
-          <a:ext cx="1181100" cy="695325"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1058" name="Picture 1" descr="SE-Logo"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="38100" y="38100"/>
-          <a:ext cx="1186016" cy="699319"/>
+          <a:ext cx="1190932" cy="699319"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2722,8 +2676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScale="93" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A10" zoomScale="93" zoomScaleNormal="100" zoomScaleSheetLayoutView="93" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2753,38 +2707,38 @@
     <row r="2" spans="1:14">
       <c r="A2" s="9"/>
       <c r="B2" s="10"/>
-      <c r="C2" s="137" t="s">
+      <c r="C2" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="137"/>
-      <c r="H2" s="137"/>
-      <c r="I2" s="137"/>
-      <c r="J2" s="137"/>
-      <c r="K2" s="137"/>
-      <c r="L2" s="137"/>
-      <c r="M2" s="137"/>
-      <c r="N2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="139"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="11"/>
       <c r="B3" s="10"/>
-      <c r="C3" s="137"/>
-      <c r="D3" s="137"/>
-      <c r="E3" s="137"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="137"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="137"/>
-      <c r="K3" s="137"/>
-      <c r="L3" s="137"/>
-      <c r="M3" s="137"/>
-      <c r="N3" s="138"/>
-    </row>
-    <row r="4" spans="1:14" ht="19.5">
+      <c r="C3" s="138"/>
+      <c r="D3" s="138"/>
+      <c r="E3" s="138"/>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="138"/>
+      <c r="N3" s="139"/>
+    </row>
+    <row r="4" spans="1:14" ht="12.75" customHeight="1">
       <c r="A4" s="11"/>
       <c r="B4" s="10"/>
       <c r="C4" s="12"/>
@@ -2802,7 +2756,7 @@
       <c r="M4" s="10"/>
       <c r="N4" s="15"/>
     </row>
-    <row r="5" spans="1:14" ht="14.25">
+    <row r="5" spans="1:14" ht="14.25" customHeight="1">
       <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
@@ -2839,108 +2793,108 @@
       <c r="N6" s="18"/>
     </row>
     <row r="7" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A7" s="139" t="s">
+      <c r="A7" s="140" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="140"/>
-      <c r="C7" s="141"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="142"/>
       <c r="D7" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="142" t="s">
+      <c r="E7" s="143" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="141"/>
-      <c r="G7" s="142" t="s">
+      <c r="F7" s="142"/>
+      <c r="G7" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="140"/>
-      <c r="I7" s="140"/>
-      <c r="J7" s="140"/>
-      <c r="K7" s="140"/>
-      <c r="L7" s="140"/>
-      <c r="M7" s="140"/>
-      <c r="N7" s="143"/>
+      <c r="H7" s="141"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="141"/>
+      <c r="N7" s="144"/>
     </row>
     <row r="8" spans="1:14" ht="13.5" customHeight="1" thickTop="1">
-      <c r="A8" s="144">
+      <c r="A8" s="145">
         <v>41459</v>
       </c>
-      <c r="B8" s="145"/>
-      <c r="C8" s="146"/>
-      <c r="D8" s="150"/>
-      <c r="E8" s="152"/>
-      <c r="F8" s="153"/>
-      <c r="G8" s="156"/>
-      <c r="H8" s="157"/>
-      <c r="I8" s="156"/>
-      <c r="J8" s="157"/>
-      <c r="K8" s="156"/>
-      <c r="L8" s="157"/>
-      <c r="M8" s="158"/>
-      <c r="N8" s="159"/>
+      <c r="B8" s="146"/>
+      <c r="C8" s="147"/>
+      <c r="D8" s="151"/>
+      <c r="E8" s="153"/>
+      <c r="F8" s="154"/>
+      <c r="G8" s="157"/>
+      <c r="H8" s="158"/>
+      <c r="I8" s="157"/>
+      <c r="J8" s="158"/>
+      <c r="K8" s="157"/>
+      <c r="L8" s="158"/>
+      <c r="M8" s="159"/>
+      <c r="N8" s="160"/>
     </row>
     <row r="9" spans="1:14" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A9" s="147"/>
-      <c r="B9" s="148"/>
-      <c r="C9" s="149"/>
-      <c r="D9" s="151"/>
-      <c r="E9" s="154"/>
-      <c r="F9" s="155"/>
-      <c r="G9" s="160"/>
-      <c r="H9" s="161"/>
-      <c r="I9" s="160"/>
-      <c r="J9" s="161"/>
-      <c r="K9" s="160"/>
-      <c r="L9" s="161"/>
-      <c r="M9" s="162"/>
-      <c r="N9" s="163"/>
+      <c r="A9" s="148"/>
+      <c r="B9" s="149"/>
+      <c r="C9" s="150"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="155"/>
+      <c r="F9" s="156"/>
+      <c r="G9" s="161"/>
+      <c r="H9" s="162"/>
+      <c r="I9" s="161"/>
+      <c r="J9" s="162"/>
+      <c r="K9" s="161"/>
+      <c r="L9" s="162"/>
+      <c r="M9" s="163"/>
+      <c r="N9" s="164"/>
     </row>
     <row r="10" spans="1:14">
-      <c r="A10" s="110" t="s">
+      <c r="A10" s="111" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="112" t="s">
+      <c r="B10" s="113" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="113"/>
-      <c r="D10" s="113"/>
-      <c r="E10" s="113"/>
-      <c r="F10" s="113"/>
-      <c r="G10" s="113"/>
-      <c r="H10" s="113"/>
-      <c r="I10" s="113"/>
-      <c r="J10" s="113"/>
-      <c r="K10" s="113"/>
-      <c r="L10" s="113"/>
-      <c r="M10" s="113"/>
-      <c r="N10" s="114"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="114"/>
+      <c r="H10" s="114"/>
+      <c r="I10" s="114"/>
+      <c r="J10" s="114"/>
+      <c r="K10" s="114"/>
+      <c r="L10" s="114"/>
+      <c r="M10" s="114"/>
+      <c r="N10" s="115"/>
     </row>
     <row r="11" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A11" s="111"/>
-      <c r="B11" s="115" t="s">
+      <c r="A11" s="112"/>
+      <c r="B11" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="116"/>
-      <c r="D11" s="116"/>
-      <c r="E11" s="116"/>
-      <c r="F11" s="116"/>
-      <c r="G11" s="116"/>
-      <c r="H11" s="116"/>
-      <c r="I11" s="116"/>
-      <c r="J11" s="117" t="s">
+      <c r="C11" s="117"/>
+      <c r="D11" s="117"/>
+      <c r="E11" s="117"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="117"/>
+      <c r="H11" s="117"/>
+      <c r="I11" s="117"/>
+      <c r="J11" s="118" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="118"/>
-      <c r="L11" s="118"/>
-      <c r="M11" s="118"/>
-      <c r="N11" s="119"/>
+      <c r="K11" s="119"/>
+      <c r="L11" s="119"/>
+      <c r="M11" s="119"/>
+      <c r="N11" s="120"/>
     </row>
     <row r="12" spans="1:14">
-      <c r="A12" s="107">
+      <c r="A12" s="108">
         <v>0.29166666666666669</v>
       </c>
-      <c r="B12" s="120" t="s">
+      <c r="B12" s="121" t="s">
         <v>12</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -2952,7 +2906,7 @@
       <c r="E12" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="120" t="s">
+      <c r="F12" s="121" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="22" t="s">
@@ -2975,8 +2929,8 @@
       <c r="N12" s="26"/>
     </row>
     <row r="13" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A13" s="108"/>
-      <c r="B13" s="121"/>
+      <c r="A13" s="109"/>
+      <c r="B13" s="122"/>
       <c r="C13" s="27" t="s">
         <v>17</v>
       </c>
@@ -2986,7 +2940,7 @@
       <c r="E13" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="F13" s="122"/>
+      <c r="F13" s="123"/>
       <c r="G13" s="28" t="s">
         <v>17</v>
       </c>
@@ -3007,7 +2961,7 @@
       <c r="N13" s="31"/>
     </row>
     <row r="14" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A14" s="108"/>
+      <c r="A14" s="109"/>
       <c r="B14" s="101"/>
       <c r="C14" s="95"/>
       <c r="D14" s="95"/>
@@ -3016,14 +2970,14 @@
       <c r="G14" s="97"/>
       <c r="H14" s="97"/>
       <c r="I14" s="99"/>
-      <c r="J14" s="201"/>
-      <c r="K14" s="202"/>
+      <c r="J14" s="202"/>
+      <c r="K14" s="203"/>
       <c r="L14" s="32"/>
       <c r="M14" s="33"/>
       <c r="N14" s="34"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1">
-      <c r="A15" s="108"/>
+      <c r="A15" s="109"/>
       <c r="B15" s="102"/>
       <c r="C15" s="95"/>
       <c r="D15" s="95"/>
@@ -3032,14 +2986,14 @@
       <c r="G15" s="96"/>
       <c r="H15" s="95"/>
       <c r="I15" s="100"/>
-      <c r="J15" s="203"/>
-      <c r="K15" s="204"/>
+      <c r="J15" s="204"/>
+      <c r="K15" s="205"/>
       <c r="L15" s="35"/>
       <c r="M15" s="36"/>
       <c r="N15" s="37"/>
     </row>
     <row r="16" spans="1:14" ht="15" customHeight="1">
-      <c r="A16" s="108"/>
+      <c r="A16" s="109"/>
       <c r="B16" s="102"/>
       <c r="C16" s="95"/>
       <c r="D16" s="95"/>
@@ -3048,14 +3002,14 @@
       <c r="G16" s="96"/>
       <c r="H16" s="95"/>
       <c r="I16" s="100"/>
-      <c r="J16" s="205"/>
-      <c r="K16" s="204"/>
+      <c r="J16" s="206"/>
+      <c r="K16" s="205"/>
       <c r="L16" s="35"/>
       <c r="M16" s="36"/>
       <c r="N16" s="37"/>
     </row>
     <row r="17" spans="1:14">
-      <c r="A17" s="108"/>
+      <c r="A17" s="109"/>
       <c r="B17" s="102"/>
       <c r="C17" s="95"/>
       <c r="D17" s="95"/>
@@ -3064,14 +3018,14 @@
       <c r="G17" s="96"/>
       <c r="H17" s="95"/>
       <c r="I17" s="100"/>
-      <c r="J17" s="205"/>
-      <c r="K17" s="204"/>
+      <c r="J17" s="206"/>
+      <c r="K17" s="205"/>
       <c r="L17" s="35"/>
       <c r="M17" s="36"/>
       <c r="N17" s="37"/>
     </row>
     <row r="18" spans="1:14">
-      <c r="A18" s="108"/>
+      <c r="A18" s="109"/>
       <c r="B18" s="102"/>
       <c r="C18" s="95"/>
       <c r="D18" s="95"/>
@@ -3080,14 +3034,14 @@
       <c r="G18" s="96"/>
       <c r="H18" s="95"/>
       <c r="I18" s="100"/>
-      <c r="J18" s="205"/>
-      <c r="K18" s="204"/>
+      <c r="J18" s="206"/>
+      <c r="K18" s="205"/>
       <c r="L18" s="35"/>
       <c r="M18" s="36"/>
       <c r="N18" s="37"/>
     </row>
     <row r="19" spans="1:14">
-      <c r="A19" s="108"/>
+      <c r="A19" s="109"/>
       <c r="B19" s="102"/>
       <c r="C19" s="95"/>
       <c r="D19" s="95"/>
@@ -3096,14 +3050,14 @@
       <c r="G19" s="96"/>
       <c r="H19" s="95"/>
       <c r="I19" s="100"/>
-      <c r="J19" s="205"/>
-      <c r="K19" s="204"/>
+      <c r="J19" s="206"/>
+      <c r="K19" s="205"/>
       <c r="L19" s="35"/>
       <c r="M19" s="36"/>
       <c r="N19" s="37"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="108"/>
+      <c r="A20" s="109"/>
       <c r="B20" s="102"/>
       <c r="C20" s="95"/>
       <c r="D20" s="95"/>
@@ -3112,14 +3066,14 @@
       <c r="G20" s="96"/>
       <c r="H20" s="95"/>
       <c r="I20" s="100"/>
-      <c r="J20" s="205"/>
-      <c r="K20" s="204"/>
+      <c r="J20" s="206"/>
+      <c r="K20" s="205"/>
       <c r="L20" s="35"/>
       <c r="M20" s="36"/>
       <c r="N20" s="37"/>
     </row>
     <row r="21" spans="1:14">
-      <c r="A21" s="108"/>
+      <c r="A21" s="109"/>
       <c r="B21" s="102"/>
       <c r="C21" s="95"/>
       <c r="D21" s="95"/>
@@ -3128,14 +3082,14 @@
       <c r="G21" s="96"/>
       <c r="H21" s="95"/>
       <c r="I21" s="100"/>
-      <c r="J21" s="205"/>
-      <c r="K21" s="204"/>
+      <c r="J21" s="206"/>
+      <c r="K21" s="205"/>
       <c r="L21" s="35"/>
       <c r="M21" s="36"/>
       <c r="N21" s="37"/>
     </row>
     <row r="22" spans="1:14">
-      <c r="A22" s="108"/>
+      <c r="A22" s="109"/>
       <c r="B22" s="102"/>
       <c r="C22" s="95"/>
       <c r="D22" s="95"/>
@@ -3144,14 +3098,14 @@
       <c r="G22" s="96"/>
       <c r="H22" s="95"/>
       <c r="I22" s="100"/>
-      <c r="J22" s="205"/>
-      <c r="K22" s="204"/>
+      <c r="J22" s="206"/>
+      <c r="K22" s="205"/>
       <c r="L22" s="35"/>
       <c r="M22" s="36"/>
       <c r="N22" s="37"/>
     </row>
     <row r="23" spans="1:14">
-      <c r="A23" s="108"/>
+      <c r="A23" s="109"/>
       <c r="B23" s="102"/>
       <c r="C23" s="95"/>
       <c r="D23" s="95"/>
@@ -3160,14 +3114,14 @@
       <c r="G23" s="96"/>
       <c r="H23" s="95"/>
       <c r="I23" s="100"/>
-      <c r="J23" s="205"/>
-      <c r="K23" s="204"/>
+      <c r="J23" s="206"/>
+      <c r="K23" s="205"/>
       <c r="L23" s="35"/>
       <c r="M23" s="36"/>
       <c r="N23" s="37"/>
     </row>
     <row r="24" spans="1:14">
-      <c r="A24" s="108"/>
+      <c r="A24" s="109"/>
       <c r="B24" s="102"/>
       <c r="C24" s="95"/>
       <c r="D24" s="95"/>
@@ -3176,14 +3130,14 @@
       <c r="G24" s="96"/>
       <c r="H24" s="95"/>
       <c r="I24" s="100"/>
-      <c r="J24" s="205"/>
-      <c r="K24" s="204"/>
+      <c r="J24" s="206"/>
+      <c r="K24" s="205"/>
       <c r="L24" s="35"/>
       <c r="M24" s="36"/>
       <c r="N24" s="37"/>
     </row>
     <row r="25" spans="1:14">
-      <c r="A25" s="108"/>
+      <c r="A25" s="109"/>
       <c r="B25" s="102"/>
       <c r="C25" s="95"/>
       <c r="D25" s="95"/>
@@ -3192,14 +3146,14 @@
       <c r="G25" s="96"/>
       <c r="H25" s="95"/>
       <c r="I25" s="100"/>
-      <c r="J25" s="205"/>
-      <c r="K25" s="204"/>
+      <c r="J25" s="206"/>
+      <c r="K25" s="205"/>
       <c r="L25" s="35"/>
       <c r="M25" s="36"/>
       <c r="N25" s="37"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="108"/>
+      <c r="A26" s="109"/>
       <c r="B26" s="102"/>
       <c r="C26" s="95"/>
       <c r="D26" s="95"/>
@@ -3208,14 +3162,14 @@
       <c r="G26" s="96"/>
       <c r="H26" s="95"/>
       <c r="I26" s="100"/>
-      <c r="J26" s="205"/>
-      <c r="K26" s="204"/>
+      <c r="J26" s="206"/>
+      <c r="K26" s="205"/>
       <c r="L26" s="35"/>
       <c r="M26" s="36"/>
       <c r="N26" s="37"/>
     </row>
     <row r="27" spans="1:14">
-      <c r="A27" s="108"/>
+      <c r="A27" s="109"/>
       <c r="B27" s="103"/>
       <c r="C27" s="95"/>
       <c r="D27" s="95"/>
@@ -3224,30 +3178,30 @@
       <c r="G27" s="96"/>
       <c r="H27" s="95"/>
       <c r="I27" s="100"/>
-      <c r="J27" s="205"/>
-      <c r="K27" s="204"/>
+      <c r="J27" s="206"/>
+      <c r="K27" s="205"/>
       <c r="L27" s="35"/>
       <c r="M27" s="36"/>
       <c r="N27" s="37"/>
     </row>
     <row r="28" spans="1:14">
-      <c r="A28" s="108"/>
+      <c r="A28" s="109"/>
       <c r="B28" s="102"/>
       <c r="C28" s="96"/>
       <c r="D28" s="97"/>
       <c r="E28" s="98"/>
       <c r="F28" s="106"/>
-      <c r="G28" s="206"/>
-      <c r="H28" s="206"/>
+      <c r="G28" s="107"/>
+      <c r="H28" s="107"/>
       <c r="I28" s="100"/>
-      <c r="J28" s="205"/>
-      <c r="K28" s="204"/>
+      <c r="J28" s="206"/>
+      <c r="K28" s="205"/>
       <c r="L28" s="35"/>
       <c r="M28" s="36"/>
       <c r="N28" s="37"/>
     </row>
     <row r="29" spans="1:14">
-      <c r="A29" s="108"/>
+      <c r="A29" s="109"/>
       <c r="B29" s="38" t="s">
         <v>22</v>
       </c>
@@ -3272,14 +3226,14 @@
       <c r="I29" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="J29" s="203"/>
-      <c r="K29" s="204"/>
+      <c r="J29" s="204"/>
+      <c r="K29" s="205"/>
       <c r="L29" s="35"/>
       <c r="M29" s="36"/>
       <c r="N29" s="37"/>
     </row>
     <row r="30" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A30" s="108"/>
+      <c r="A30" s="109"/>
       <c r="B30" s="40" t="s">
         <v>30</v>
       </c>
@@ -3304,14 +3258,14 @@
       <c r="I30" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="J30" s="203"/>
-      <c r="K30" s="204"/>
+      <c r="J30" s="204"/>
+      <c r="K30" s="205"/>
       <c r="L30" s="35"/>
       <c r="M30" s="36"/>
       <c r="N30" s="37"/>
     </row>
     <row r="31" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A31" s="108"/>
+      <c r="A31" s="109"/>
       <c r="B31" s="42"/>
       <c r="C31" s="42"/>
       <c r="D31" s="42"/>
@@ -3320,14 +3274,14 @@
       <c r="G31" s="42"/>
       <c r="H31" s="42"/>
       <c r="I31" s="43"/>
-      <c r="J31" s="203"/>
-      <c r="K31" s="204"/>
+      <c r="J31" s="204"/>
+      <c r="K31" s="205"/>
       <c r="L31" s="35"/>
       <c r="M31" s="36"/>
       <c r="N31" s="37"/>
     </row>
     <row r="32" spans="1:14">
-      <c r="A32" s="108"/>
+      <c r="A32" s="109"/>
       <c r="B32" s="44" t="s">
         <v>34</v>
       </c>
@@ -3352,14 +3306,14 @@
       <c r="I32" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="J32" s="203"/>
-      <c r="K32" s="204"/>
+      <c r="J32" s="204"/>
+      <c r="K32" s="205"/>
       <c r="L32" s="35"/>
       <c r="M32" s="36"/>
       <c r="N32" s="37"/>
     </row>
     <row r="33" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A33" s="108"/>
+      <c r="A33" s="109"/>
       <c r="B33" s="40" t="s">
         <v>42</v>
       </c>
@@ -3384,14 +3338,14 @@
       <c r="I33" s="47" t="s">
         <v>42</v>
       </c>
-      <c r="J33" s="203"/>
-      <c r="K33" s="204"/>
+      <c r="J33" s="204"/>
+      <c r="K33" s="205"/>
       <c r="L33" s="35"/>
       <c r="M33" s="36"/>
       <c r="N33" s="37"/>
     </row>
     <row r="34" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A34" s="108"/>
+      <c r="A34" s="109"/>
       <c r="B34" s="48"/>
       <c r="C34" s="48"/>
       <c r="D34" s="48"/>
@@ -3400,43 +3354,43 @@
       <c r="G34" s="48"/>
       <c r="H34" s="49"/>
       <c r="I34" s="43"/>
-      <c r="J34" s="203"/>
-      <c r="K34" s="204"/>
+      <c r="J34" s="204"/>
+      <c r="K34" s="205"/>
       <c r="L34" s="50"/>
       <c r="M34" s="51"/>
       <c r="N34" s="52"/>
     </row>
     <row r="35" spans="1:14">
-      <c r="A35" s="108"/>
-      <c r="B35" s="123" t="s">
+      <c r="A35" s="109"/>
+      <c r="B35" s="124" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="124"/>
-      <c r="D35" s="124"/>
-      <c r="E35" s="124"/>
-      <c r="F35" s="124"/>
-      <c r="G35" s="124"/>
-      <c r="H35" s="124"/>
-      <c r="I35" s="124"/>
-      <c r="J35" s="125"/>
-      <c r="K35" s="125"/>
-      <c r="L35" s="124"/>
-      <c r="M35" s="124"/>
-      <c r="N35" s="126"/>
+      <c r="C35" s="125"/>
+      <c r="D35" s="125"/>
+      <c r="E35" s="125"/>
+      <c r="F35" s="125"/>
+      <c r="G35" s="125"/>
+      <c r="H35" s="125"/>
+      <c r="I35" s="125"/>
+      <c r="J35" s="126"/>
+      <c r="K35" s="126"/>
+      <c r="L35" s="125"/>
+      <c r="M35" s="125"/>
+      <c r="N35" s="127"/>
     </row>
     <row r="36" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A36" s="108"/>
+      <c r="A36" s="109"/>
       <c r="B36" s="53"/>
       <c r="C36" s="54"/>
       <c r="D36" s="53"/>
-      <c r="E36" s="127" t="s">
+      <c r="E36" s="128" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="128"/>
-      <c r="G36" s="129" t="s">
+      <c r="F36" s="129"/>
+      <c r="G36" s="130" t="s">
         <v>21</v>
       </c>
-      <c r="H36" s="130"/>
+      <c r="H36" s="131"/>
       <c r="I36" s="55"/>
       <c r="J36" s="56"/>
       <c r="K36" s="57"/>
@@ -3449,7 +3403,7 @@
       <c r="N36" s="60"/>
     </row>
     <row r="37" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A37" s="108"/>
+      <c r="A37" s="109"/>
       <c r="B37" s="61" t="s">
         <v>48</v>
       </c>
@@ -3457,10 +3411,10 @@
       <c r="D37" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="E37" s="131"/>
-      <c r="F37" s="132"/>
-      <c r="G37" s="131"/>
-      <c r="H37" s="132"/>
+      <c r="E37" s="132"/>
+      <c r="F37" s="133"/>
+      <c r="G37" s="132"/>
+      <c r="H37" s="133"/>
       <c r="I37" s="64" t="s">
         <v>50</v>
       </c>
@@ -3475,7 +3429,7 @@
       </c>
     </row>
     <row r="38" spans="1:14">
-      <c r="A38" s="108"/>
+      <c r="A38" s="109"/>
       <c r="B38" s="69" t="s">
         <v>52</v>
       </c>
@@ -3483,10 +3437,10 @@
       <c r="D38" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="E38" s="133"/>
-      <c r="F38" s="134"/>
-      <c r="G38" s="133"/>
-      <c r="H38" s="134"/>
+      <c r="E38" s="134"/>
+      <c r="F38" s="135"/>
+      <c r="G38" s="134"/>
+      <c r="H38" s="135"/>
       <c r="I38" s="72" t="s">
         <v>54</v>
       </c>
@@ -3501,7 +3455,7 @@
       </c>
     </row>
     <row r="39" spans="1:14">
-      <c r="A39" s="108"/>
+      <c r="A39" s="109"/>
       <c r="B39" s="76" t="s">
         <v>56</v>
       </c>
@@ -3509,10 +3463,10 @@
       <c r="D39" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="E39" s="135"/>
-      <c r="F39" s="136"/>
-      <c r="G39" s="135"/>
-      <c r="H39" s="136"/>
+      <c r="E39" s="136"/>
+      <c r="F39" s="137"/>
+      <c r="G39" s="136"/>
+      <c r="H39" s="137"/>
       <c r="I39" s="64" t="s">
         <v>58</v>
       </c>
@@ -3527,7 +3481,7 @@
       </c>
     </row>
     <row r="40" spans="1:14">
-      <c r="A40" s="108"/>
+      <c r="A40" s="109"/>
       <c r="B40" s="69" t="s">
         <v>60</v>
       </c>
@@ -3535,10 +3489,10 @@
       <c r="D40" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="164"/>
-      <c r="F40" s="165"/>
-      <c r="G40" s="166"/>
-      <c r="H40" s="167"/>
+      <c r="E40" s="165"/>
+      <c r="F40" s="166"/>
+      <c r="G40" s="167"/>
+      <c r="H40" s="168"/>
       <c r="I40" s="79" t="s">
         <v>58</v>
       </c>
@@ -3553,17 +3507,17 @@
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A41" s="108"/>
-      <c r="B41" s="168" t="s">
+      <c r="A41" s="109"/>
+      <c r="B41" s="169" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="169"/>
-      <c r="D41" s="169"/>
-      <c r="E41" s="169"/>
-      <c r="F41" s="169"/>
-      <c r="G41" s="169"/>
-      <c r="H41" s="169"/>
-      <c r="I41" s="170"/>
+      <c r="C41" s="170"/>
+      <c r="D41" s="170"/>
+      <c r="E41" s="170"/>
+      <c r="F41" s="170"/>
+      <c r="G41" s="170"/>
+      <c r="H41" s="170"/>
+      <c r="I41" s="171"/>
       <c r="J41" s="73" t="s">
         <v>64</v>
       </c>
@@ -3575,18 +3529,18 @@
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A42" s="108"/>
-      <c r="B42" s="171" t="s">
+      <c r="A42" s="109"/>
+      <c r="B42" s="172" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="172"/>
+      <c r="C42" s="173"/>
       <c r="D42" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="E42" s="131"/>
-      <c r="F42" s="132"/>
-      <c r="G42" s="173"/>
-      <c r="H42" s="174"/>
+      <c r="E42" s="132"/>
+      <c r="F42" s="133"/>
+      <c r="G42" s="174"/>
+      <c r="H42" s="175"/>
       <c r="I42" s="64" t="s">
         <v>50</v>
       </c>
@@ -3601,7 +3555,7 @@
       </c>
     </row>
     <row r="43" spans="1:14" ht="13.5" thickBot="1">
-      <c r="A43" s="108"/>
+      <c r="A43" s="109"/>
       <c r="B43" s="84" t="s">
         <v>67</v>
       </c>
@@ -3609,23 +3563,23 @@
       <c r="D43" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="E43" s="133"/>
-      <c r="F43" s="134"/>
-      <c r="G43" s="175"/>
-      <c r="H43" s="176"/>
+      <c r="E43" s="134"/>
+      <c r="F43" s="135"/>
+      <c r="G43" s="176"/>
+      <c r="H43" s="177"/>
       <c r="I43" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="J43" s="129" t="s">
+      <c r="J43" s="130" t="s">
         <v>68</v>
       </c>
-      <c r="K43" s="189"/>
-      <c r="L43" s="189"/>
-      <c r="M43" s="189"/>
-      <c r="N43" s="190"/>
+      <c r="K43" s="190"/>
+      <c r="L43" s="190"/>
+      <c r="M43" s="190"/>
+      <c r="N43" s="191"/>
     </row>
     <row r="44" spans="1:14" ht="13.5" thickTop="1">
-      <c r="A44" s="108"/>
+      <c r="A44" s="109"/>
       <c r="B44" s="76" t="s">
         <v>69</v>
       </c>
@@ -3633,10 +3587,10 @@
       <c r="D44" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="191"/>
-      <c r="F44" s="192"/>
-      <c r="G44" s="193"/>
-      <c r="H44" s="194"/>
+      <c r="E44" s="192"/>
+      <c r="F44" s="193"/>
+      <c r="G44" s="194"/>
+      <c r="H44" s="195"/>
       <c r="I44" s="64" t="s">
         <v>50</v>
       </c>
@@ -3651,16 +3605,16 @@
       </c>
     </row>
     <row r="45" spans="1:14">
-      <c r="A45" s="108"/>
+      <c r="A45" s="109"/>
       <c r="B45" s="69"/>
       <c r="C45" s="70"/>
       <c r="D45" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="E45" s="195"/>
-      <c r="F45" s="196"/>
-      <c r="G45" s="197"/>
-      <c r="H45" s="198"/>
+      <c r="E45" s="196"/>
+      <c r="F45" s="197"/>
+      <c r="G45" s="198"/>
+      <c r="H45" s="199"/>
       <c r="I45" s="87" t="s">
         <v>50</v>
       </c>
@@ -3675,7 +3629,7 @@
       </c>
     </row>
     <row r="46" spans="1:14">
-      <c r="A46" s="108"/>
+      <c r="A46" s="109"/>
       <c r="B46" s="76" t="s">
         <v>74</v>
       </c>
@@ -3683,10 +3637,10 @@
       <c r="D46" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="E46" s="199"/>
-      <c r="F46" s="200"/>
-      <c r="G46" s="199"/>
-      <c r="H46" s="200"/>
+      <c r="E46" s="200"/>
+      <c r="F46" s="201"/>
+      <c r="G46" s="200"/>
+      <c r="H46" s="201"/>
       <c r="I46" s="64" t="s">
         <v>58</v>
       </c>
@@ -3701,29 +3655,29 @@
       </c>
     </row>
     <row r="47" spans="1:14">
-      <c r="A47" s="108"/>
+      <c r="A47" s="109"/>
       <c r="B47" s="69"/>
       <c r="C47" s="70"/>
       <c r="D47" s="86" t="s">
         <v>77</v>
       </c>
-      <c r="E47" s="177"/>
-      <c r="F47" s="178"/>
-      <c r="G47" s="178"/>
-      <c r="H47" s="179"/>
+      <c r="E47" s="178"/>
+      <c r="F47" s="179"/>
+      <c r="G47" s="179"/>
+      <c r="H47" s="180"/>
       <c r="I47" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="J47" s="180" t="s">
+      <c r="J47" s="181" t="s">
         <v>78</v>
       </c>
-      <c r="K47" s="181"/>
-      <c r="L47" s="181"/>
-      <c r="M47" s="181"/>
-      <c r="N47" s="182"/>
+      <c r="K47" s="182"/>
+      <c r="L47" s="182"/>
+      <c r="M47" s="182"/>
+      <c r="N47" s="183"/>
     </row>
     <row r="48" spans="1:14">
-      <c r="A48" s="109"/>
+      <c r="A48" s="110"/>
       <c r="B48" s="91" t="s">
         <v>79</v>
       </c>
@@ -3731,18 +3685,18 @@
       <c r="D48" s="93" t="s">
         <v>77</v>
       </c>
-      <c r="E48" s="183"/>
-      <c r="F48" s="184"/>
-      <c r="G48" s="184"/>
-      <c r="H48" s="185"/>
+      <c r="E48" s="184"/>
+      <c r="F48" s="185"/>
+      <c r="G48" s="185"/>
+      <c r="H48" s="186"/>
       <c r="I48" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="J48" s="186"/>
-      <c r="K48" s="187"/>
-      <c r="L48" s="187"/>
-      <c r="M48" s="187"/>
-      <c r="N48" s="188"/>
+      <c r="J48" s="187"/>
+      <c r="K48" s="188"/>
+      <c r="L48" s="188"/>
+      <c r="M48" s="188"/>
+      <c r="N48" s="189"/>
     </row>
   </sheetData>
   <mergeCells count="71">

</xml_diff>